<commit_message>
Added the results xls. Plus multiple test out files
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="38480" yWindow="0" windowWidth="25600" windowHeight="22760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Testnummer</t>
   </si>
@@ -52,6 +52,84 @@
   </si>
   <si>
     <t>Size Output</t>
+  </si>
+  <si>
+    <t>Dop</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>2,67 GB</t>
+  </si>
+  <si>
+    <t>01:00:30h</t>
+  </si>
+  <si>
+    <t>00:58:44h</t>
+  </si>
+  <si>
+    <t>02:11m</t>
+  </si>
+  <si>
+    <t>01:58m</t>
+  </si>
+  <si>
+    <t>01:50m</t>
+  </si>
+  <si>
+    <t>02:32:46h</t>
+  </si>
+  <si>
+    <t>02:19:45h</t>
+  </si>
+  <si>
+    <t>02:18:20h</t>
+  </si>
+  <si>
+    <t>00:59:28h</t>
+  </si>
+  <si>
+    <t>02:29:50h</t>
+  </si>
+  <si>
+    <t>02:17:47h</t>
+  </si>
+  <si>
+    <t>01:29:55h</t>
+  </si>
+  <si>
+    <t>01:20:15h</t>
+  </si>
+  <si>
+    <t>01:12:51h</t>
+  </si>
+  <si>
+    <t>02:16:28h</t>
+  </si>
+  <si>
+    <t>00:46:38h</t>
+  </si>
+  <si>
+    <t>01:55m</t>
+  </si>
+  <si>
+    <t>00:18:31h</t>
+  </si>
+  <si>
+    <t>00:44:36h</t>
+  </si>
+  <si>
+    <t>00:27:52h</t>
+  </si>
+  <si>
+    <t>2,7GB</t>
   </si>
 </sst>
 </file>
@@ -87,8 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -420,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -432,15 +513,16 @@
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -457,22 +539,205 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>337</v>
+      </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>144</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>337</v>
+      </c>
+      <c r="D3">
+        <v>500</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>144</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>337</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>144</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>337</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>144</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>337</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>337</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented the satelliteAnalysis.py Improved the thesis
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
   <si>
     <t>Testnummer</t>
   </si>
@@ -220,6 +220,66 @@
   </si>
   <si>
     <t>01:05:40h</t>
+  </si>
+  <si>
+    <t>01:02:40h</t>
+  </si>
+  <si>
+    <t>01:38m</t>
+  </si>
+  <si>
+    <t>00:03:26h</t>
+  </si>
+  <si>
+    <t>00:59:36h</t>
+  </si>
+  <si>
+    <t>01:00:55h</t>
+  </si>
+  <si>
+    <t>01:03:20h</t>
+  </si>
+  <si>
+    <t>01:43m</t>
+  </si>
+  <si>
+    <t>01:01:30h</t>
+  </si>
+  <si>
+    <t>00:58:53h</t>
+  </si>
+  <si>
+    <t>00:04:18h</t>
+  </si>
+  <si>
+    <t>02:23:56h</t>
+  </si>
+  <si>
+    <t>03:18m</t>
+  </si>
+  <si>
+    <t>00:05:14h</t>
+  </si>
+  <si>
+    <t>02:18:35h</t>
+  </si>
+  <si>
+    <t>02:20:36h</t>
+  </si>
+  <si>
+    <t>02:26:06h</t>
+  </si>
+  <si>
+    <t>01:46m</t>
+  </si>
+  <si>
+    <t>00:02:53h</t>
+  </si>
+  <si>
+    <t>02:24:12h</t>
+  </si>
+  <si>
+    <t>02:23:04h</t>
   </si>
 </sst>
 </file>
@@ -591,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1064,6 +1124,24 @@
       <c r="F15">
         <v>144</v>
       </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" t="s">
@@ -1079,6 +1157,117 @@
         <v>100</v>
       </c>
       <c r="F16">
+        <v>144</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" t="s">
+        <v>75</v>
+      </c>
+      <c r="L16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>337</v>
+      </c>
+      <c r="D18">
+        <v>500</v>
+      </c>
+      <c r="E18">
+        <v>250</v>
+      </c>
+      <c r="F18">
+        <v>144</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>337</v>
+      </c>
+      <c r="D19">
+        <v>500</v>
+      </c>
+      <c r="E19">
+        <v>250</v>
+      </c>
+      <c r="F19">
+        <v>144</v>
+      </c>
+      <c r="G19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" t="s">
+        <v>84</v>
+      </c>
+      <c r="J19" t="s">
+        <v>85</v>
+      </c>
+      <c r="K19" t="s">
+        <v>86</v>
+      </c>
+      <c r="L19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>337</v>
+      </c>
+      <c r="D20">
+        <v>500</v>
+      </c>
+      <c r="E20">
+        <v>250</v>
+      </c>
+      <c r="F20">
         <v>144</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved the thesis, eradicated OLS, have a functioning python program
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
   <si>
     <t>Testnummer</t>
   </si>
@@ -280,16 +280,77 @@
   </si>
   <si>
     <t>02:23:04h</t>
+  </si>
+  <si>
+    <t>02:25:51h</t>
+  </si>
+  <si>
+    <t>01:56m</t>
+  </si>
+  <si>
+    <t>00:02:49h</t>
+  </si>
+  <si>
+    <t>02:22:54h</t>
+  </si>
+  <si>
+    <t>02:23:47h</t>
+  </si>
+  <si>
+    <t>02:14m</t>
+  </si>
+  <si>
+    <t>00:03:58h</t>
+  </si>
+  <si>
+    <t>05:50:16h</t>
+  </si>
+  <si>
+    <t>05:52:03h</t>
+  </si>
+  <si>
+    <t>2,72GB</t>
+  </si>
+  <si>
+    <t>05:54:23h</t>
+  </si>
+  <si>
+    <t>05:56:52h</t>
+  </si>
+  <si>
+    <t>00:04:40h</t>
+  </si>
+  <si>
+    <t>01:52m</t>
+  </si>
+  <si>
+    <t>05:54:54h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -312,8 +373,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -321,7 +390,15 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -651,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -664,7 +741,7 @@
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
@@ -1142,6 +1219,9 @@
       <c r="L15" t="s">
         <v>51</v>
       </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" t="s">
@@ -1177,6 +1257,9 @@
       <c r="L16" t="s">
         <v>51</v>
       </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18">
@@ -1215,6 +1298,9 @@
       <c r="L18" t="s">
         <v>51</v>
       </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:13">
       <c r="B19" t="s">
@@ -1270,9 +1356,189 @@
       <c r="F20">
         <v>144</v>
       </c>
+      <c r="G20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" t="s">
+        <v>90</v>
+      </c>
+      <c r="L20" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>337</v>
+      </c>
+      <c r="D22">
+        <v>500</v>
+      </c>
+      <c r="E22">
+        <v>500</v>
+      </c>
+      <c r="F22">
+        <v>144</v>
+      </c>
+      <c r="G22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22" t="s">
+        <v>95</v>
+      </c>
+      <c r="K22" t="s">
+        <v>94</v>
+      </c>
+      <c r="L22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>337</v>
+      </c>
+      <c r="D23">
+        <v>500</v>
+      </c>
+      <c r="E23">
+        <v>500</v>
+      </c>
+      <c r="F23">
+        <v>144</v>
+      </c>
+      <c r="G23" t="s">
+        <v>98</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>337</v>
+      </c>
+      <c r="D24">
+        <v>500</v>
+      </c>
+      <c r="E24">
+        <v>500</v>
+      </c>
+      <c r="F24">
+        <v>144</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>337</v>
+      </c>
+      <c r="D26">
+        <v>2000</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="F26">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>337</v>
+      </c>
+      <c r="D27">
+        <v>2000</v>
+      </c>
+      <c r="E27">
+        <v>50</v>
+      </c>
+      <c r="F27">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>337</v>
+      </c>
+      <c r="D28">
+        <v>2000</v>
+      </c>
+      <c r="E28">
+        <v>50</v>
+      </c>
+      <c r="F28">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Started working on the complexity analysis
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="0" windowWidth="25600" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="113">
   <si>
     <t>Testnummer</t>
   </si>
@@ -150,6 +150,9 @@
     <t>00:47:35h</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>00:28:47h</t>
   </si>
   <si>
@@ -325,6 +328,36 @@
   </si>
   <si>
     <t>05:54:54h</t>
+  </si>
+  <si>
+    <t>02:36:33h</t>
+  </si>
+  <si>
+    <t>10,9GB</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>02:54m</t>
+  </si>
+  <si>
+    <t>00:54:00h</t>
+  </si>
+  <si>
+    <t>02:13:27h</t>
+  </si>
+  <si>
+    <t>40:51m</t>
+  </si>
+  <si>
+    <t>02:40:51h</t>
   </si>
 </sst>
 </file>
@@ -384,11 +417,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -728,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -787,7 +821,7 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1006,16 +1040,16 @@
         <v>42</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="I8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="L8" t="s">
         <v>36</v>
@@ -1044,22 +1078,22 @@
         <v>144</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" t="s">
         <v>52</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" t="s">
-        <v>51</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1082,22 +1116,22 @@
         <v>144</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1120,22 +1154,22 @@
         <v>144</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1164,22 +1198,22 @@
         <v>144</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K14" t="s">
         <v>16</v>
       </c>
       <c r="L14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -1202,22 +1236,22 @@
         <v>144</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J15" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" t="s">
         <v>71</v>
       </c>
-      <c r="K15" t="s">
-        <v>70</v>
-      </c>
       <c r="L15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1240,22 +1274,22 @@
         <v>144</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" t="s">
         <v>76</v>
       </c>
-      <c r="J16" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" t="s">
-        <v>75</v>
-      </c>
       <c r="L16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -1281,22 +1315,22 @@
         <v>144</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s">
+        <v>82</v>
+      </c>
+      <c r="K18" t="s">
         <v>81</v>
       </c>
-      <c r="K18" t="s">
-        <v>80</v>
-      </c>
       <c r="L18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1319,22 +1353,22 @@
         <v>144</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -1357,22 +1391,22 @@
         <v>144</v>
       </c>
       <c r="G20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" t="s">
         <v>91</v>
       </c>
-      <c r="K20" t="s">
-        <v>90</v>
-      </c>
       <c r="L20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -1398,22 +1432,22 @@
         <v>144</v>
       </c>
       <c r="G22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" t="s">
+        <v>95</v>
+      </c>
+      <c r="L22" t="s">
         <v>97</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22" t="s">
-        <v>95</v>
-      </c>
-      <c r="K22" t="s">
-        <v>94</v>
-      </c>
-      <c r="L22" t="s">
-        <v>96</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -1436,22 +1470,22 @@
         <v>144</v>
       </c>
       <c r="G23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" t="s">
         <v>100</v>
       </c>
-      <c r="I23" t="s">
-        <v>99</v>
-      </c>
       <c r="J23" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -1488,13 +1522,34 @@
         <v>337</v>
       </c>
       <c r="D26">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E26">
         <v>50</v>
       </c>
       <c r="F26">
         <v>144</v>
+      </c>
+      <c r="G26" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" t="s">
+        <v>108</v>
+      </c>
+      <c r="I26" t="s">
+        <v>109</v>
+      </c>
+      <c r="J26" t="s">
+        <v>110</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L26" t="s">
+        <v>104</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1505,7 +1560,7 @@
         <v>337</v>
       </c>
       <c r="D27">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E27">
         <v>50</v>
@@ -1522,7 +1577,7 @@
         <v>337</v>
       </c>
       <c r="D28">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E28">
         <v>50</v>
@@ -1535,6 +1590,56 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.69170138888888888</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.69371527777777775</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.69171296296296303</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.72921296296296301</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.70761574074074074</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.8002893518518519</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.56041666666666667</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.73025462962962961</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.8002893518518519</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finished the complexityAnalysis. Added new results.
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
   <si>
     <t>Testnummer</t>
   </si>
@@ -354,7 +354,37 @@
     <t>02:13:27h</t>
   </si>
   <si>
-    <t>02:40:51h</t>
+    <t>02:31:11h</t>
+  </si>
+  <si>
+    <t>04:05m</t>
+  </si>
+  <si>
+    <t>00:51:01h</t>
+  </si>
+  <si>
+    <t>02:26:05h</t>
+  </si>
+  <si>
+    <t>01:48:12h</t>
+  </si>
+  <si>
+    <t>01:40:51h</t>
+  </si>
+  <si>
+    <t>02:31:07h</t>
+  </si>
+  <si>
+    <t>03:35m</t>
+  </si>
+  <si>
+    <t>00:40:34h</t>
+  </si>
+  <si>
+    <t>02:27:22h</t>
+  </si>
+  <si>
+    <t>02:39:05h</t>
   </si>
 </sst>
 </file>
@@ -414,12 +444,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -762,7 +791,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1540,7 +1569,7 @@
         <v>110</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="L26" t="s">
         <v>104</v>
@@ -1565,6 +1594,27 @@
       <c r="F27">
         <v>144</v>
       </c>
+      <c r="G27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J27" t="s">
+        <v>114</v>
+      </c>
+      <c r="K27" t="s">
+        <v>115</v>
+      </c>
+      <c r="L27" t="s">
+        <v>104</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:13">
       <c r="B28" t="s">
@@ -1581,6 +1631,27 @@
       </c>
       <c r="F28">
         <v>144</v>
+      </c>
+      <c r="G28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" t="s">
+        <v>119</v>
+      </c>
+      <c r="J28" t="s">
+        <v>120</v>
+      </c>
+      <c r="K28" t="s">
+        <v>121</v>
+      </c>
+      <c r="L28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1595,14 +1666,14 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="3:6">
+    <row r="33" spans="3:7">
       <c r="C33" t="s">
         <v>106</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="3:6">
+    <row r="34" spans="3:7">
       <c r="C34" t="s">
         <v>43</v>
       </c>
@@ -1610,13 +1681,14 @@
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="3:6">
+    <row r="35" spans="3:7">
       <c r="C35" t="s">
         <v>107</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="4"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added new results. Worked on part 4
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16660" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="0" windowWidth="16720" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="370">
   <si>
     <t>Testnummer</t>
   </si>
@@ -706,6 +706,9 @@
     <t>00:12:43h</t>
   </si>
   <si>
+    <t>4:56m</t>
+  </si>
+  <si>
     <t>00:07m</t>
   </si>
   <si>
@@ -758,6 +761,375 @@
   </si>
   <si>
     <t>05:14m</t>
+  </si>
+  <si>
+    <t>05:27m</t>
+  </si>
+  <si>
+    <t>00:09m</t>
+  </si>
+  <si>
+    <t>03:58m</t>
+  </si>
+  <si>
+    <t>01:22m</t>
+  </si>
+  <si>
+    <t>05:41m</t>
+  </si>
+  <si>
+    <t>00:08m</t>
+  </si>
+  <si>
+    <t>03:46m</t>
+  </si>
+  <si>
+    <t>05:29m</t>
+  </si>
+  <si>
+    <t>01:48m</t>
+  </si>
+  <si>
+    <t>09:48m</t>
+  </si>
+  <si>
+    <t>00:20m</t>
+  </si>
+  <si>
+    <t>07:18m</t>
+  </si>
+  <si>
+    <t>09:26m</t>
+  </si>
+  <si>
+    <t>02:25m</t>
+  </si>
+  <si>
+    <t>11:15m</t>
+  </si>
+  <si>
+    <t>00:17m</t>
+  </si>
+  <si>
+    <t>07:42m</t>
+  </si>
+  <si>
+    <t>10:53m</t>
+  </si>
+  <si>
+    <t>03:16m</t>
+  </si>
+  <si>
+    <t>08:47m</t>
+  </si>
+  <si>
+    <t>00:35m</t>
+  </si>
+  <si>
+    <t>06:35m</t>
+  </si>
+  <si>
+    <t>08:08m</t>
+  </si>
+  <si>
+    <t>02:04m</t>
+  </si>
+  <si>
+    <t>00:48m</t>
+  </si>
+  <si>
+    <t>08:24m</t>
+  </si>
+  <si>
+    <t>12:38m</t>
+  </si>
+  <si>
+    <t>13:29m</t>
+  </si>
+  <si>
+    <t>13:54m</t>
+  </si>
+  <si>
+    <t>00:41m</t>
+  </si>
+  <si>
+    <t>08:45m</t>
+  </si>
+  <si>
+    <t>13:07m</t>
+  </si>
+  <si>
+    <t>5:00m</t>
+  </si>
+  <si>
+    <t>12:47m</t>
+  </si>
+  <si>
+    <t>00:47m</t>
+  </si>
+  <si>
+    <t>07:49m</t>
+  </si>
+  <si>
+    <t>11:55m</t>
+  </si>
+  <si>
+    <t>4:49m</t>
+  </si>
+  <si>
+    <t>00:14:22h</t>
+  </si>
+  <si>
+    <t>00:02:26h</t>
+  </si>
+  <si>
+    <t>00:12:07h</t>
+  </si>
+  <si>
+    <t>00:11:48h</t>
+  </si>
+  <si>
+    <t>45:30m</t>
+  </si>
+  <si>
+    <t>01:35m</t>
+  </si>
+  <si>
+    <t>16:14m</t>
+  </si>
+  <si>
+    <t>43:45m</t>
+  </si>
+  <si>
+    <t>28:14m</t>
+  </si>
+  <si>
+    <t>46:26m</t>
+  </si>
+  <si>
+    <t>01:40m</t>
+  </si>
+  <si>
+    <t>17:35m</t>
+  </si>
+  <si>
+    <t>44:38m</t>
+  </si>
+  <si>
+    <t>27:38m</t>
+  </si>
+  <si>
+    <t>01:05:43h</t>
+  </si>
+  <si>
+    <t>01:29m</t>
+  </si>
+  <si>
+    <t>18:49m</t>
+  </si>
+  <si>
+    <t>46:07m</t>
+  </si>
+  <si>
+    <t>01:04:07h</t>
+  </si>
+  <si>
+    <t>48:57m</t>
+  </si>
+  <si>
+    <t>01:28m</t>
+  </si>
+  <si>
+    <t>17:51m</t>
+  </si>
+  <si>
+    <t>47:21m</t>
+  </si>
+  <si>
+    <t>29:59m</t>
+  </si>
+  <si>
+    <t>01:02:59h</t>
+  </si>
+  <si>
+    <t>01:26m</t>
+  </si>
+  <si>
+    <t>16:16m</t>
+  </si>
+  <si>
+    <t>01:01:26h</t>
+  </si>
+  <si>
+    <t>45:59m</t>
+  </si>
+  <si>
+    <t>01:03:19h</t>
+  </si>
+  <si>
+    <t>01:27m</t>
+  </si>
+  <si>
+    <t>16:36m</t>
+  </si>
+  <si>
+    <t>01:01:45h</t>
+  </si>
+  <si>
+    <t>45:37m</t>
+  </si>
+  <si>
+    <t>06:33m</t>
+  </si>
+  <si>
+    <t>00:51m</t>
+  </si>
+  <si>
+    <t>05:35m</t>
+  </si>
+  <si>
+    <t>02:51m</t>
+  </si>
+  <si>
+    <t>00:49m</t>
+  </si>
+  <si>
+    <t>08:20m</t>
+  </si>
+  <si>
+    <t>03:57m</t>
+  </si>
+  <si>
+    <t>06:19m</t>
+  </si>
+  <si>
+    <t>02:27m</t>
+  </si>
+  <si>
+    <t>08:12m</t>
+  </si>
+  <si>
+    <t>01:00m</t>
+  </si>
+  <si>
+    <t>03:25m</t>
+  </si>
+  <si>
+    <t>07:01m</t>
+  </si>
+  <si>
+    <t>05:53m</t>
+  </si>
+  <si>
+    <t>01:24m</t>
+  </si>
+  <si>
+    <t>04:19m</t>
+  </si>
+  <si>
+    <t>02:16m</t>
+  </si>
+  <si>
+    <t>05:08m</t>
+  </si>
+  <si>
+    <t>04:07m</t>
+  </si>
+  <si>
+    <t>01:42m</t>
+  </si>
+  <si>
+    <t>06:32m</t>
+  </si>
+  <si>
+    <t>01:25m</t>
+  </si>
+  <si>
+    <t>02:42m</t>
+  </si>
+  <si>
+    <t>06:07m</t>
+  </si>
+  <si>
+    <t>02:31m</t>
+  </si>
+  <si>
+    <t>05:17m</t>
+  </si>
+  <si>
+    <t>00:53m</t>
+  </si>
+  <si>
+    <t>03:21m</t>
+  </si>
+  <si>
+    <t>02:30m</t>
+  </si>
+  <si>
+    <t>01:11m</t>
+  </si>
+  <si>
+    <t>05:25m</t>
+  </si>
+  <si>
+    <t>02:49m</t>
+  </si>
+  <si>
+    <t>04:10m</t>
+  </si>
+  <si>
+    <t>00:36m</t>
+  </si>
+  <si>
+    <t>03:15m</t>
+  </si>
+  <si>
+    <t>02:09m</t>
+  </si>
+  <si>
+    <t>00:26m</t>
+  </si>
+  <si>
+    <t>01:36m</t>
+  </si>
+  <si>
+    <t>00:45m</t>
+  </si>
+  <si>
+    <t>00:46m</t>
+  </si>
+  <si>
+    <t>02:35m</t>
+  </si>
+  <si>
+    <t>9b</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>Py - a</t>
+  </si>
+  <si>
+    <t>Py - b</t>
+  </si>
+  <si>
+    <t>Py - c</t>
+  </si>
+  <si>
+    <t>Py -a</t>
+  </si>
+  <si>
+    <t>9c</t>
+  </si>
+  <si>
+    <t>00:05m</t>
+  </si>
+  <si>
+    <t>01:06m</t>
+  </si>
+  <si>
+    <t>00:37m</t>
   </si>
 </sst>
 </file>
@@ -796,7 +1168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -806,6 +1178,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,7 +1197,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -857,8 +1235,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -866,8 +1258,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="46" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="51">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -886,6 +1285,13 @@
     <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -904,6 +1310,13 @@
     <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1233,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S136"/>
+  <dimension ref="A1:T154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I88" workbookViewId="0">
-      <selection activeCell="N112" sqref="N112"/>
+    <sheetView tabSelected="1" topLeftCell="I106" workbookViewId="0">
+      <selection activeCell="S128" sqref="S128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1330,40 +1743,41 @@
       <c r="F2">
         <v>144</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="9">
         <v>0</v>
       </c>
-      <c r="O2">
+      <c r="N2" s="9"/>
+      <c r="O2" s="9">
         <v>9166</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="9">
         <v>131</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="9">
         <v>3630</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="9">
         <v>8990</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="9">
         <v>5395</v>
       </c>
     </row>
@@ -1386,40 +1800,41 @@
       <c r="F3">
         <v>144</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="9">
         <v>0</v>
       </c>
-      <c r="O3">
+      <c r="N3" s="9"/>
+      <c r="O3" s="9">
         <v>8385</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="9">
         <v>118</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="9">
         <v>3524</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="9">
         <v>8267</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="9">
         <v>4815</v>
       </c>
     </row>
@@ -1439,40 +1854,41 @@
       <c r="F4">
         <v>144</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="9">
         <v>0</v>
       </c>
-      <c r="O4">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9">
         <v>8300</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="9">
         <v>110</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="9">
         <v>3568</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="9">
         <v>8188</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="9">
         <v>4371</v>
       </c>
     </row>
@@ -1618,34 +2034,37 @@
       <c r="B8" t="s">
         <v>157</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="O8">
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9">
         <v>8617</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="9">
         <v>120</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="9">
         <v>3574</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="9">
         <v>8482</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="9">
         <v>4860</v>
       </c>
     </row>
@@ -1693,40 +2112,41 @@
       <c r="F11">
         <v>144</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="9">
         <v>0</v>
       </c>
-      <c r="O11">
+      <c r="N11" s="9"/>
+      <c r="O11" s="9">
         <v>2798</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="9">
         <v>115</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="9">
         <v>1111</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="9">
         <v>2676</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="9">
         <v>1672</v>
       </c>
     </row>
@@ -1749,40 +2169,41 @@
       <c r="F12">
         <v>144</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="9">
         <v>0</v>
       </c>
-      <c r="O12">
+      <c r="N12" s="9"/>
+      <c r="O12" s="9">
         <v>2837</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="9">
         <v>168</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="9">
         <v>1112</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="9">
         <v>2663</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="9">
         <v>1712</v>
       </c>
     </row>
@@ -1802,40 +2223,41 @@
       <c r="F13">
         <v>144</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="9">
         <v>0</v>
       </c>
-      <c r="O13">
+      <c r="N13" s="9"/>
+      <c r="O13" s="9">
         <v>2855</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="9">
         <v>159</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="9">
         <v>1114</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="9">
         <v>2808</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="9">
         <v>1227</v>
       </c>
     </row>
@@ -2002,21 +2424,27 @@
       <c r="F17">
         <v>144</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="K17" s="2"/>
-      <c r="O17">
+      <c r="G17" s="9"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9">
         <v>2830</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="9">
         <v>147</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="9">
         <v>1112</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="9">
         <v>2716</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="9">
         <v>1522</v>
       </c>
     </row>
@@ -2073,40 +2501,41 @@
       <c r="F20">
         <v>144</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K20" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="9">
         <v>0</v>
       </c>
-      <c r="O20">
+      <c r="N20" s="9"/>
+      <c r="O20" s="9">
         <v>2447</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="9">
         <v>99</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="9">
         <v>311</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="9">
         <v>2342</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="9">
         <v>2127</v>
       </c>
     </row>
@@ -2129,40 +2558,41 @@
       <c r="F21">
         <v>144</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="9">
         <v>0</v>
       </c>
-      <c r="O21">
+      <c r="N21" s="9"/>
+      <c r="O21" s="9">
         <v>2323</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="9">
         <v>104</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="9">
         <v>333</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="9">
         <v>2213</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="9">
         <v>1982</v>
       </c>
     </row>
@@ -2182,40 +2612,41 @@
       <c r="F22">
         <v>144</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="9">
         <v>0</v>
       </c>
-      <c r="O22">
+      <c r="N22" s="9"/>
+      <c r="O22" s="9">
         <v>2615</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="9">
         <v>143</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="9">
         <v>526</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="9">
         <v>2464</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="9">
         <v>2080</v>
       </c>
     </row>
@@ -2373,20 +2804,27 @@
       <c r="B26" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="O26">
+      <c r="G26" s="9"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9">
         <v>2462</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="9">
         <v>115</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="9">
         <v>390</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="9">
         <v>2340</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="9">
         <v>2063</v>
       </c>
     </row>
@@ -2433,40 +2871,41 @@
       <c r="F29">
         <v>144</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="9">
         <v>1</v>
       </c>
-      <c r="O29">
+      <c r="N29" s="9"/>
+      <c r="O29" s="9">
         <v>4058</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="9">
         <v>110</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="9">
         <v>418</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="9">
         <v>3960</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="9">
         <v>3630</v>
       </c>
     </row>
@@ -2489,40 +2928,41 @@
       <c r="F30">
         <v>144</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="9">
         <v>0</v>
       </c>
-      <c r="O30">
+      <c r="N30" s="9"/>
+      <c r="O30" s="9">
         <v>3760</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="9">
         <v>98</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="9">
         <v>206</v>
       </c>
-      <c r="R30">
+      <c r="R30" s="9">
         <v>3655</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="9">
         <v>3576</v>
       </c>
     </row>
@@ -2542,40 +2982,41 @@
       <c r="F31">
         <v>144</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I31" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L31" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="9">
         <v>0</v>
       </c>
-      <c r="O31">
+      <c r="N31" s="9"/>
+      <c r="O31" s="9">
         <v>3800</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="9">
         <v>103</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="9">
         <v>258</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="9">
         <v>3690</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="9">
         <v>3533</v>
       </c>
     </row>
@@ -2693,21 +3134,27 @@
       <c r="B35" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="O35">
+      <c r="G35" s="9"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9">
         <v>3873</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="9">
         <v>104</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="9">
         <v>294</v>
       </c>
-      <c r="R35">
+      <c r="R35" s="9">
         <v>3768</v>
       </c>
-      <c r="S35">
+      <c r="S35" s="9">
         <v>3580</v>
       </c>
     </row>
@@ -2737,40 +3184,41 @@
       <c r="F38">
         <v>144</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="9">
         <v>0</v>
       </c>
-      <c r="O38">
+      <c r="N38" s="9"/>
+      <c r="O38" s="9">
         <v>8636</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="9">
         <v>198</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="9">
         <v>314</v>
       </c>
-      <c r="R38">
+      <c r="R38" s="9">
         <v>8436</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="9">
         <v>8315</v>
       </c>
     </row>
@@ -2793,40 +3241,41 @@
       <c r="F39">
         <v>144</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L39" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="9">
         <v>1</v>
       </c>
-      <c r="O39">
+      <c r="N39" s="9"/>
+      <c r="O39" s="9">
         <v>8766</v>
       </c>
-      <c r="P39">
+      <c r="P39" s="9">
         <v>106</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="9">
         <v>173</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="9">
         <v>8652</v>
       </c>
-      <c r="S39">
+      <c r="S39" s="9">
         <v>8584</v>
       </c>
     </row>
@@ -2846,40 +3295,41 @@
       <c r="F40">
         <v>144</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K40" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L40" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="9">
         <v>1</v>
       </c>
-      <c r="O40">
+      <c r="N40" s="9"/>
+      <c r="O40" s="9">
         <v>8751</v>
       </c>
-      <c r="P40">
+      <c r="P40" s="9">
         <v>116</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="9">
         <v>169</v>
       </c>
-      <c r="R40">
+      <c r="R40" s="9">
         <v>8627</v>
       </c>
-      <c r="S40">
+      <c r="S40" s="9">
         <v>8574</v>
       </c>
     </row>
@@ -2917,20 +3367,27 @@
       <c r="B44" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H44" s="1"/>
-      <c r="O44">
+      <c r="G44" s="9"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9">
         <v>8718</v>
       </c>
-      <c r="P44">
+      <c r="P44" s="9">
         <v>140</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="9">
         <v>219</v>
       </c>
-      <c r="R44">
+      <c r="R44" s="9">
         <v>8572</v>
       </c>
-      <c r="S44">
+      <c r="S44" s="9">
         <v>8491</v>
       </c>
     </row>
@@ -2962,26 +3419,42 @@
       <c r="F47">
         <v>144</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K47" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="L47" t="s">
+      <c r="L47" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="9">
         <v>1</v>
+      </c>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9">
+        <v>21263</v>
+      </c>
+      <c r="P47" s="9">
+        <v>134</v>
+      </c>
+      <c r="Q47" s="9">
+        <v>238</v>
+      </c>
+      <c r="R47" s="9">
+        <v>21123</v>
+      </c>
+      <c r="S47" s="9">
+        <v>21016</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -3003,26 +3476,42 @@
       <c r="F48">
         <v>144</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="K48" t="s">
+      <c r="K48" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="L48" t="s">
+      <c r="L48" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="9">
         <v>0</v>
+      </c>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9">
+        <v>21412</v>
+      </c>
+      <c r="P48" s="9">
+        <v>112</v>
+      </c>
+      <c r="Q48" s="9">
+        <v>280</v>
+      </c>
+      <c r="R48" s="9">
+        <v>21294</v>
+      </c>
+      <c r="S48" s="9">
+        <v>21123</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -3041,9 +3530,21 @@
       <c r="F49">
         <v>144</v>
       </c>
-      <c r="M49">
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9">
         <v>1</v>
       </c>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
     </row>
     <row r="50" spans="1:19">
       <c r="B50" s="4" t="s">
@@ -3069,121 +3570,35 @@
         <v>181</v>
       </c>
     </row>
+    <row r="53" spans="1:19">
+      <c r="B53" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
+    </row>
     <row r="54" spans="1:19">
-      <c r="A54">
+      <c r="B54" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="A56">
         <v>7</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>12</v>
-      </c>
-      <c r="C54">
-        <v>373</v>
-      </c>
-      <c r="D54">
-        <v>1000</v>
-      </c>
-      <c r="E54">
-        <v>50</v>
-      </c>
-      <c r="F54">
-        <v>144</v>
-      </c>
-      <c r="G54" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" t="s">
-        <v>104</v>
-      </c>
-      <c r="I54" t="s">
-        <v>105</v>
-      </c>
-      <c r="J54" t="s">
-        <v>106</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L54" t="s">
-        <v>103</v>
-      </c>
-      <c r="M54">
-        <v>1</v>
-      </c>
-      <c r="O54">
-        <v>9393</v>
-      </c>
-      <c r="P54">
-        <v>174</v>
-      </c>
-      <c r="Q54">
-        <v>3240</v>
-      </c>
-      <c r="R54">
-        <v>8007</v>
-      </c>
-      <c r="S54">
-        <v>6051</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19">
-      <c r="A55" t="s">
-        <v>203</v>
-      </c>
-      <c r="B55" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55">
-        <v>373</v>
-      </c>
-      <c r="D55">
-        <v>1000</v>
-      </c>
-      <c r="E55">
-        <v>50</v>
-      </c>
-      <c r="F55">
-        <v>144</v>
-      </c>
-      <c r="G55" t="s">
-        <v>107</v>
-      </c>
-      <c r="H55" t="s">
-        <v>108</v>
-      </c>
-      <c r="I55" t="s">
-        <v>109</v>
-      </c>
-      <c r="J55" t="s">
-        <v>110</v>
-      </c>
-      <c r="K55" t="s">
-        <v>111</v>
-      </c>
-      <c r="L55" t="s">
-        <v>103</v>
-      </c>
-      <c r="M55">
-        <v>1</v>
-      </c>
-      <c r="O55">
-        <v>9071</v>
-      </c>
-      <c r="P55">
-        <v>245</v>
-      </c>
-      <c r="Q55">
-        <v>3061</v>
-      </c>
-      <c r="R55">
-        <v>8765</v>
-      </c>
-      <c r="S55">
-        <v>6492</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="B56" t="s">
-        <v>14</v>
       </c>
       <c r="C56">
         <v>373</v>
@@ -3197,68 +3612,181 @@
       <c r="F56">
         <v>144</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L56" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="M56" s="9">
+        <v>1</v>
+      </c>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9">
+        <v>9393</v>
+      </c>
+      <c r="P56" s="9">
+        <v>174</v>
+      </c>
+      <c r="Q56" s="9">
+        <v>3240</v>
+      </c>
+      <c r="R56" s="9">
+        <v>8007</v>
+      </c>
+      <c r="S56" s="9">
+        <v>6051</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
+      <c r="A57" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57">
+        <v>373</v>
+      </c>
+      <c r="D57">
+        <v>1000</v>
+      </c>
+      <c r="E57">
+        <v>50</v>
+      </c>
+      <c r="F57">
+        <v>144</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="L57" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="M57" s="9">
+        <v>1</v>
+      </c>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9">
+        <v>9071</v>
+      </c>
+      <c r="P57" s="9">
+        <v>245</v>
+      </c>
+      <c r="Q57" s="9">
+        <v>3061</v>
+      </c>
+      <c r="R57" s="9">
+        <v>8765</v>
+      </c>
+      <c r="S57" s="9">
+        <v>6492</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>373</v>
+      </c>
+      <c r="D58">
+        <v>1000</v>
+      </c>
+      <c r="E58">
+        <v>50</v>
+      </c>
+      <c r="F58">
+        <v>144</v>
+      </c>
+      <c r="G58" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H58" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I58" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J58" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="K56" t="s">
-        <v>237</v>
-      </c>
-      <c r="L56" t="s">
+      <c r="K58" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="L58" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="M56">
+      <c r="M58" s="9">
         <v>0</v>
       </c>
-      <c r="O56">
+      <c r="N58" s="9"/>
+      <c r="O58" s="9">
         <v>9067</v>
       </c>
-      <c r="P56">
+      <c r="P58" s="9">
         <v>215</v>
       </c>
-      <c r="Q56">
+      <c r="Q58" s="9">
         <v>2434</v>
       </c>
-      <c r="R56">
+      <c r="R58" s="9">
         <v>8842</v>
       </c>
-      <c r="S56">
+      <c r="S58" s="9">
         <v>5945</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19">
-      <c r="B57" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G57" t="s">
-        <v>181</v>
-      </c>
-      <c r="M57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="B58" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G58" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:19">
       <c r="B59" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G59" t="s">
-        <v>181</v>
+        <v>157</v>
+      </c>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="O59" s="9">
+        <v>9177</v>
+      </c>
+      <c r="P59" s="9">
+        <v>211</v>
+      </c>
+      <c r="Q59" s="9">
+        <v>2912</v>
+      </c>
+      <c r="R59" s="9">
+        <v>8538</v>
+      </c>
+      <c r="S59" s="9">
+        <v>6163</v>
       </c>
     </row>
     <row r="61" spans="1:19">
@@ -3280,37 +3808,39 @@
       <c r="F61" s="5">
         <v>144</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="G61" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H61" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K61" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="M61">
+      <c r="L61" s="9"/>
+      <c r="M61" s="9">
         <v>0</v>
       </c>
-      <c r="O61">
+      <c r="N61" s="9"/>
+      <c r="O61" s="9">
         <v>1090</v>
       </c>
-      <c r="P61">
+      <c r="P61" s="9">
         <v>68</v>
       </c>
-      <c r="Q61">
+      <c r="Q61" s="9">
         <v>117</v>
       </c>
-      <c r="R61">
+      <c r="R61" s="9">
         <v>1014</v>
       </c>
-      <c r="S61">
+      <c r="S61" s="9">
         <v>966</v>
       </c>
     </row>
@@ -3333,37 +3863,39 @@
       <c r="F62" s="5">
         <v>144</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="G62" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I62" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="J62" s="5" t="s">
+      <c r="J62" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="K62" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="M62">
+      <c r="L62" s="9"/>
+      <c r="M62" s="9">
         <v>0</v>
       </c>
-      <c r="O62">
+      <c r="N62" s="9"/>
+      <c r="O62" s="9">
         <v>847</v>
       </c>
-      <c r="P62">
+      <c r="P62" s="9">
         <v>65</v>
       </c>
-      <c r="Q62">
+      <c r="Q62" s="9">
         <v>75</v>
       </c>
-      <c r="R62">
+      <c r="R62" s="9">
         <v>774</v>
       </c>
-      <c r="S62">
+      <c r="S62" s="9">
         <v>763</v>
       </c>
     </row>
@@ -3383,11 +3915,40 @@
       <c r="F63" s="5">
         <v>144</v>
       </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="M63">
-        <v>1</v>
+      <c r="G63" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9">
+        <v>2</v>
+      </c>
+      <c r="N63" s="9"/>
+      <c r="O63" s="9">
+        <v>862</v>
+      </c>
+      <c r="P63" s="9">
+        <v>126</v>
+      </c>
+      <c r="Q63" s="9">
+        <v>146</v>
+      </c>
+      <c r="R63" s="9">
+        <v>727</v>
+      </c>
+      <c r="S63" s="9">
+        <v>708</v>
       </c>
     </row>
     <row r="64" spans="1:19">
@@ -3397,9 +3958,29 @@
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9">
+        <v>933</v>
+      </c>
+      <c r="P64" s="9">
+        <v>86</v>
+      </c>
+      <c r="Q64" s="9">
+        <v>113</v>
+      </c>
+      <c r="R64" s="9">
+        <v>838</v>
+      </c>
+      <c r="S64" s="9">
+        <v>812</v>
+      </c>
     </row>
     <row r="65" spans="1:19">
       <c r="B65" s="4"/>
@@ -3429,9 +4010,19 @@
       <c r="F66" s="5">
         <v>1</v>
       </c>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+      <c r="O66" s="9"/>
+      <c r="P66" s="9"/>
+      <c r="Q66" s="9"/>
+      <c r="R66" s="9"/>
+      <c r="S66" s="9"/>
     </row>
     <row r="67" spans="1:19">
       <c r="A67" t="s">
@@ -3443,9 +4034,19 @@
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="O67" s="9"/>
+      <c r="P67" s="9"/>
+      <c r="Q67" s="9"/>
+      <c r="R67" s="9"/>
+      <c r="S67" s="9"/>
     </row>
     <row r="68" spans="1:19">
       <c r="B68" s="4" t="s">
@@ -3454,9 +4055,19 @@
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="9"/>
+      <c r="S68" s="9"/>
     </row>
     <row r="69" spans="1:19">
       <c r="B69" s="4" t="s">
@@ -3513,9 +4124,19 @@
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+      <c r="O72" s="9"/>
+      <c r="P72" s="9"/>
+      <c r="Q72" s="9"/>
+      <c r="R72" s="9"/>
+      <c r="S72" s="9"/>
     </row>
     <row r="73" spans="1:19">
       <c r="B73" s="4" t="s">
@@ -3529,6 +4150,7 @@
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:19">
+      <c r="B74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -3537,8 +4159,8 @@
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:19">
-      <c r="A75">
-        <v>9</v>
+      <c r="A75" t="s">
+        <v>361</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>12</v>
@@ -3553,7 +4175,7 @@
         <v>20</v>
       </c>
       <c r="F75" s="5">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
@@ -3566,18 +4188,9 @@
       <c r="B76" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C76">
-        <v>373</v>
-      </c>
-      <c r="D76" s="5">
-        <v>500</v>
-      </c>
-      <c r="E76" s="5">
-        <v>20</v>
-      </c>
-      <c r="F76" s="5">
-        <v>50</v>
-      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
@@ -3586,154 +4199,49 @@
       <c r="B77" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C77">
-        <v>373</v>
-      </c>
-      <c r="D77" s="5">
-        <v>500</v>
-      </c>
-      <c r="E77" s="5">
-        <v>20</v>
-      </c>
-      <c r="F77" s="5">
-        <v>50</v>
-      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="1:19">
       <c r="B78" s="4" t="s">
-        <v>117</v>
+        <v>362</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
-      <c r="G78" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="H78" s="1">
-        <v>8.0555555555555561E-2</v>
-      </c>
-      <c r="I78" s="1">
-        <v>0.19722222222222222</v>
-      </c>
-      <c r="J78" s="1">
-        <v>0.5625</v>
-      </c>
-      <c r="K78" s="1">
-        <v>0.25069444444444444</v>
-      </c>
-      <c r="L78" s="5"/>
-      <c r="M78" s="5">
-        <v>0</v>
-      </c>
-      <c r="N78" s="5"/>
-      <c r="O78" s="5">
-        <v>972</v>
-      </c>
-      <c r="P78" s="5">
-        <v>116</v>
-      </c>
-      <c r="Q78" s="5">
-        <v>284</v>
-      </c>
-      <c r="R78" s="5">
-        <v>810</v>
-      </c>
-      <c r="S78" s="5">
-        <v>361</v>
-      </c>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:19">
       <c r="B79" s="4" t="s">
-        <v>123</v>
+        <v>363</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
-      <c r="G79" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="H79" s="1">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="I79" s="1">
-        <v>0.21388888888888891</v>
-      </c>
-      <c r="J79" s="1">
-        <v>0.57916666666666672</v>
-      </c>
-      <c r="K79" s="1">
-        <v>0.27430555555555552</v>
-      </c>
-      <c r="L79" s="5"/>
-      <c r="M79" s="5">
-        <v>0</v>
-      </c>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5">
-        <v>1023</v>
-      </c>
-      <c r="P79">
-        <v>110</v>
-      </c>
-      <c r="Q79">
-        <v>308</v>
-      </c>
-      <c r="R79">
-        <v>834</v>
-      </c>
-      <c r="S79">
-        <v>395</v>
-      </c>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:19">
       <c r="B80" s="4" t="s">
-        <v>124</v>
+        <v>364</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
-      <c r="G80" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H80" s="1">
-        <v>7.6388888888888895E-2</v>
-      </c>
-      <c r="I80" s="1">
-        <v>0.18541666666666667</v>
-      </c>
-      <c r="J80" s="1">
-        <v>0.56111111111111112</v>
-      </c>
-      <c r="K80" s="1">
-        <v>0.20972222222222223</v>
-      </c>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5">
-        <v>0</v>
-      </c>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5">
-        <v>948</v>
-      </c>
-      <c r="P80">
-        <v>110</v>
-      </c>
-      <c r="Q80">
-        <v>267</v>
-      </c>
-      <c r="R80">
-        <v>808</v>
-      </c>
-      <c r="S80">
-        <v>302</v>
-      </c>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
     </row>
     <row r="81" spans="1:19">
       <c r="B81" s="4" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
@@ -3744,7 +4252,7 @@
     </row>
     <row r="82" spans="1:19">
       <c r="B82" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
@@ -3752,12 +4260,10 @@
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
-      <c r="O82">
-        <v>981</v>
-      </c>
     </row>
     <row r="83" spans="1:19">
       <c r="B83" s="4"/>
+      <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
@@ -3765,8 +4271,8 @@
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="1:19">
-      <c r="A84">
-        <v>10</v>
+      <c r="A84" t="s">
+        <v>360</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>12</v>
@@ -3774,15 +4280,18 @@
       <c r="C84">
         <v>373</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="5">
         <v>500</v>
       </c>
       <c r="E84" s="5">
         <v>20</v>
       </c>
       <c r="F84" s="5">
-        <v>100</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
     </row>
     <row r="85" spans="1:19">
       <c r="A85" t="s">
@@ -3791,176 +4300,90 @@
       <c r="B85" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C85">
-        <v>373</v>
-      </c>
-      <c r="D85">
-        <v>500</v>
-      </c>
-      <c r="E85" s="5">
-        <v>20</v>
-      </c>
-      <c r="F85" s="5">
-        <v>100</v>
-      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
     </row>
     <row r="86" spans="1:19">
       <c r="B86" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C86">
-        <v>373</v>
-      </c>
-      <c r="D86">
-        <v>500</v>
-      </c>
-      <c r="E86" s="5">
-        <v>20</v>
-      </c>
-      <c r="F86" s="5">
-        <v>100</v>
-      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
     </row>
     <row r="87" spans="1:19">
       <c r="B87" s="4" t="s">
-        <v>117</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
-      <c r="G87" t="s">
-        <v>196</v>
-      </c>
-      <c r="H87" t="s">
-        <v>197</v>
-      </c>
-      <c r="I87" t="s">
-        <v>198</v>
-      </c>
-      <c r="J87" t="s">
-        <v>199</v>
-      </c>
-      <c r="K87" t="s">
-        <v>200</v>
-      </c>
-      <c r="M87">
-        <v>0</v>
-      </c>
-      <c r="O87">
-        <v>1009</v>
-      </c>
-      <c r="P87">
-        <v>103</v>
-      </c>
-      <c r="Q87">
-        <v>372</v>
-      </c>
-      <c r="R87">
-        <v>870</v>
-      </c>
-      <c r="S87">
-        <v>600</v>
-      </c>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
     </row>
     <row r="88" spans="1:19">
       <c r="B88" s="4" t="s">
-        <v>123</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
-      <c r="G88" t="s">
-        <v>205</v>
-      </c>
-      <c r="H88" t="s">
-        <v>206</v>
-      </c>
-      <c r="I88" t="s">
-        <v>207</v>
-      </c>
-      <c r="J88" t="s">
-        <v>208</v>
-      </c>
-      <c r="K88" t="s">
-        <v>209</v>
-      </c>
-      <c r="M88">
-        <v>0</v>
-      </c>
-      <c r="O88">
-        <v>1017</v>
-      </c>
-      <c r="P88">
-        <v>112</v>
-      </c>
-      <c r="Q88">
-        <v>266</v>
-      </c>
-      <c r="R88">
-        <v>888</v>
-      </c>
-      <c r="S88">
-        <v>430</v>
-      </c>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
     </row>
     <row r="89" spans="1:19">
       <c r="B89" s="4" t="s">
-        <v>124</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
-      <c r="G89" t="s">
-        <v>210</v>
-      </c>
-      <c r="H89" t="s">
-        <v>211</v>
-      </c>
-      <c r="I89" t="s">
-        <v>212</v>
-      </c>
-      <c r="J89" t="s">
-        <v>213</v>
-      </c>
-      <c r="K89" t="s">
-        <v>214</v>
-      </c>
-      <c r="M89">
-        <v>8</v>
-      </c>
-      <c r="O89">
-        <v>1137</v>
-      </c>
-      <c r="P89">
-        <v>215</v>
-      </c>
-      <c r="Q89">
-        <v>705</v>
-      </c>
-      <c r="R89">
-        <v>830</v>
-      </c>
-      <c r="S89">
-        <v>426</v>
-      </c>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
     </row>
     <row r="90" spans="1:19">
       <c r="B90" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
     </row>
     <row r="91" spans="1:19">
       <c r="B91" s="4" t="s">
-        <v>174</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="D91" s="5"/>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
-      <c r="O91">
-        <v>1054</v>
-      </c>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="1:19">
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
     </row>
     <row r="93" spans="1:19">
-      <c r="A93">
-        <v>11</v>
+      <c r="A93" t="s">
+        <v>366</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>12</v>
@@ -3968,23 +4391,49 @@
       <c r="C93">
         <v>373</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="5">
         <v>500</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="5">
         <v>20</v>
       </c>
-      <c r="F93">
-        <v>200</v>
-      </c>
-      <c r="G93" t="s">
-        <v>181</v>
-      </c>
-      <c r="H93" t="s">
-        <v>181</v>
-      </c>
-      <c r="M93">
-        <v>2</v>
+      <c r="F93" s="5">
+        <v>50</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="H93" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="I93" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="K93" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9">
+        <v>0</v>
+      </c>
+      <c r="N93" s="9"/>
+      <c r="O93" s="9">
+        <v>3943</v>
+      </c>
+      <c r="P93" s="9">
+        <v>89</v>
+      </c>
+      <c r="Q93" s="9">
+        <v>1129</v>
+      </c>
+      <c r="R93" s="9">
+        <v>3847</v>
+      </c>
+      <c r="S93" s="9">
+        <v>2767</v>
       </c>
     </row>
     <row r="94" spans="1:19">
@@ -3997,21 +4446,40 @@
       <c r="C94">
         <v>373</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="5">
         <v>500</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="5">
         <v>20</v>
       </c>
-      <c r="F94">
-        <v>200</v>
-      </c>
-      <c r="G94" t="s">
-        <v>181</v>
-      </c>
-      <c r="H94" t="s">
-        <v>181</v>
-      </c>
+      <c r="F94" s="5">
+        <v>50</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="I94" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="J94" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="K94" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L94" s="9"/>
+      <c r="M94" s="9">
+        <v>0</v>
+      </c>
+      <c r="N94" s="9"/>
+      <c r="O94" s="9"/>
+      <c r="P94" s="9"/>
+      <c r="Q94" s="9"/>
+      <c r="R94" s="9"/>
+      <c r="S94" s="9"/>
     </row>
     <row r="95" spans="1:19">
       <c r="B95" s="4" t="s">
@@ -4020,198 +4488,568 @@
       <c r="C95">
         <v>373</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="5">
         <v>500</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="5">
         <v>20</v>
       </c>
-      <c r="F95">
-        <v>200</v>
-      </c>
-      <c r="G95" t="s">
-        <v>181</v>
-      </c>
-      <c r="H95" t="s">
-        <v>181</v>
-      </c>
+      <c r="F95" s="5">
+        <v>50</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="H95" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="I95" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="J95" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="L95" s="9"/>
+      <c r="M95" s="9">
+        <v>0</v>
+      </c>
+      <c r="N95" s="9"/>
+      <c r="O95" s="9"/>
+      <c r="P95" s="9"/>
+      <c r="Q95" s="9"/>
+      <c r="R95" s="9"/>
+      <c r="S95" s="9"/>
     </row>
     <row r="96" spans="1:19">
       <c r="B96" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H96" s="1">
+        <v>8.0555555555555561E-2</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0.19722222222222222</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="K96" s="1">
+        <v>0.25069444444444444</v>
+      </c>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5">
+        <v>0</v>
+      </c>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5">
+        <v>972</v>
+      </c>
+      <c r="P96" s="5">
+        <v>116</v>
+      </c>
+      <c r="Q96" s="5">
+        <v>284</v>
+      </c>
+      <c r="R96" s="5">
+        <v>810</v>
+      </c>
+      <c r="S96" s="5">
+        <v>361</v>
+      </c>
     </row>
     <row r="97" spans="1:19">
       <c r="B97" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="H97" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0.21388888888888891</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="K97" s="1">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5">
+        <v>0</v>
+      </c>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5">
+        <v>1023</v>
+      </c>
+      <c r="P97">
+        <v>110</v>
+      </c>
+      <c r="Q97">
+        <v>308</v>
+      </c>
+      <c r="R97">
+        <v>834</v>
+      </c>
+      <c r="S97">
+        <v>395</v>
+      </c>
     </row>
     <row r="98" spans="1:19">
       <c r="B98" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="H98" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0.18541666666666667</v>
+      </c>
+      <c r="J98" s="1">
+        <v>0.56111111111111112</v>
+      </c>
+      <c r="K98" s="1">
+        <v>0.20972222222222223</v>
+      </c>
+      <c r="L98" s="5"/>
+      <c r="M98" s="5">
+        <v>0</v>
+      </c>
+      <c r="N98" s="5"/>
+      <c r="O98" s="5">
+        <v>948</v>
+      </c>
+      <c r="P98">
+        <v>110</v>
+      </c>
+      <c r="Q98">
+        <v>267</v>
+      </c>
+      <c r="R98">
+        <v>808</v>
+      </c>
+      <c r="S98">
+        <v>302</v>
+      </c>
     </row>
     <row r="99" spans="1:19">
       <c r="B99" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="9"/>
+      <c r="O99" s="9"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="9"/>
+      <c r="R99" s="9"/>
+      <c r="S99" s="9"/>
     </row>
     <row r="100" spans="1:19">
       <c r="B100" s="4" t="s">
-        <v>174</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="O100">
+        <v>981</v>
+      </c>
+      <c r="P100">
+        <v>112</v>
+      </c>
+      <c r="Q100">
+        <v>286</v>
+      </c>
+      <c r="R100">
+        <v>817</v>
+      </c>
+      <c r="S100">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19">
+      <c r="B101" s="4"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="5"/>
     </row>
     <row r="102" spans="1:19">
       <c r="A102">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C102">
-        <v>20</v>
+        <v>373</v>
       </c>
       <c r="D102">
         <v>500</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="5">
         <v>20</v>
       </c>
-      <c r="F102">
-        <v>144</v>
-      </c>
-      <c r="G102" t="s">
-        <v>236</v>
-      </c>
-      <c r="H102" t="s">
-        <v>228</v>
-      </c>
-      <c r="I102" t="s">
-        <v>229</v>
-      </c>
-      <c r="J102" t="s">
-        <v>230</v>
-      </c>
-      <c r="K102" t="s">
-        <v>231</v>
-      </c>
-      <c r="M102">
+      <c r="F102" s="5">
+        <v>100</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="H102" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="I102" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="J102" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="K102" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="L102" s="9"/>
+      <c r="M102" s="9">
         <v>0</v>
       </c>
-      <c r="O102">
-        <v>296</v>
-      </c>
-      <c r="P102">
-        <v>7</v>
-      </c>
-      <c r="Q102">
-        <v>220</v>
-      </c>
-      <c r="R102">
-        <v>287</v>
-      </c>
-      <c r="S102">
-        <v>73</v>
+      <c r="N102" s="9"/>
+      <c r="O102" s="9">
+        <v>2730</v>
+      </c>
+      <c r="P102" s="9">
+        <v>95</v>
+      </c>
+      <c r="Q102" s="9">
+        <v>974</v>
+      </c>
+      <c r="R102" s="9">
+        <v>2625</v>
+      </c>
+      <c r="S102" s="9">
+        <v>1694</v>
       </c>
     </row>
     <row r="103" spans="1:19">
       <c r="A103" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G103" t="s">
-        <v>232</v>
-      </c>
-      <c r="H103" t="s">
-        <v>228</v>
-      </c>
-      <c r="I103" t="s">
-        <v>233</v>
-      </c>
-      <c r="J103" t="s">
-        <v>235</v>
-      </c>
-      <c r="K103" t="s">
-        <v>234</v>
-      </c>
-      <c r="M103">
+      <c r="C103">
+        <v>373</v>
+      </c>
+      <c r="D103">
+        <v>500</v>
+      </c>
+      <c r="E103" s="5">
+        <v>20</v>
+      </c>
+      <c r="F103" s="5">
+        <v>100</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="H103" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="I103" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="J103" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="K103" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="L103" s="9"/>
+      <c r="M103" s="9">
         <v>0</v>
       </c>
-      <c r="O103">
-        <v>298</v>
-      </c>
-      <c r="P103">
-        <v>7</v>
-      </c>
-      <c r="Q103">
-        <v>173</v>
-      </c>
-      <c r="R103">
-        <v>289</v>
-      </c>
-      <c r="S103">
-        <v>61</v>
+      <c r="N103" s="9"/>
+      <c r="O103" s="9">
+        <v>2786</v>
+      </c>
+      <c r="P103" s="9">
+        <v>100</v>
+      </c>
+      <c r="Q103" s="9">
+        <v>1055</v>
+      </c>
+      <c r="R103" s="9">
+        <v>2678</v>
+      </c>
+      <c r="S103" s="9">
+        <v>1658</v>
       </c>
     </row>
     <row r="104" spans="1:19">
       <c r="B104" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G104" t="s">
-        <v>238</v>
-      </c>
-      <c r="H104" t="s">
-        <v>239</v>
-      </c>
-      <c r="I104" t="s">
-        <v>240</v>
-      </c>
-      <c r="J104" t="s">
-        <v>108</v>
-      </c>
-      <c r="K104" t="s">
-        <v>241</v>
-      </c>
-      <c r="M104">
+      <c r="C104">
+        <v>373</v>
+      </c>
+      <c r="D104">
+        <v>500</v>
+      </c>
+      <c r="E104" s="5">
+        <v>20</v>
+      </c>
+      <c r="F104" s="5">
+        <v>100</v>
+      </c>
+      <c r="G104" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="H104" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="I104" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="J104" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="K104" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="L104" s="9"/>
+      <c r="M104" s="9">
         <v>0</v>
+      </c>
+      <c r="N104" s="9"/>
+      <c r="O104" s="9">
+        <v>2937</v>
+      </c>
+      <c r="P104" s="9">
+        <v>88</v>
+      </c>
+      <c r="Q104" s="9">
+        <v>1071</v>
+      </c>
+      <c r="R104" s="9">
+        <v>2841</v>
+      </c>
+      <c r="S104" s="9">
+        <v>1799</v>
       </c>
     </row>
     <row r="105" spans="1:19">
       <c r="B105" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" t="s">
+        <v>196</v>
+      </c>
+      <c r="H105" t="s">
+        <v>197</v>
+      </c>
+      <c r="I105" t="s">
+        <v>198</v>
+      </c>
+      <c r="J105" t="s">
+        <v>199</v>
+      </c>
+      <c r="K105" t="s">
+        <v>200</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+      <c r="O105">
+        <v>1009</v>
+      </c>
+      <c r="P105">
+        <v>103</v>
+      </c>
+      <c r="Q105">
+        <v>372</v>
+      </c>
+      <c r="R105">
+        <v>870</v>
+      </c>
+      <c r="S105">
+        <v>600</v>
+      </c>
     </row>
     <row r="106" spans="1:19">
       <c r="B106" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" t="s">
+        <v>205</v>
+      </c>
+      <c r="H106" t="s">
+        <v>206</v>
+      </c>
+      <c r="I106" t="s">
+        <v>207</v>
+      </c>
+      <c r="J106" t="s">
+        <v>208</v>
+      </c>
+      <c r="K106" t="s">
+        <v>209</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="O106">
+        <v>1017</v>
+      </c>
+      <c r="P106">
+        <v>112</v>
+      </c>
+      <c r="Q106">
+        <v>266</v>
+      </c>
+      <c r="R106">
+        <v>888</v>
+      </c>
+      <c r="S106">
+        <v>430</v>
+      </c>
     </row>
     <row r="107" spans="1:19">
       <c r="B107" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" t="s">
+        <v>210</v>
+      </c>
+      <c r="H107" t="s">
+        <v>211</v>
+      </c>
+      <c r="I107" t="s">
+        <v>212</v>
+      </c>
+      <c r="J107" t="s">
+        <v>213</v>
+      </c>
+      <c r="K107" t="s">
+        <v>214</v>
+      </c>
+      <c r="M107">
+        <v>8</v>
+      </c>
+      <c r="O107">
+        <v>1137</v>
+      </c>
+      <c r="P107">
+        <v>215</v>
+      </c>
+      <c r="Q107">
+        <v>705</v>
+      </c>
+      <c r="R107">
+        <v>830</v>
+      </c>
+      <c r="S107">
+        <v>426</v>
+      </c>
     </row>
     <row r="108" spans="1:19">
       <c r="B108" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
+      <c r="L108" s="9"/>
+      <c r="M108" s="9"/>
+      <c r="N108" s="9"/>
+      <c r="O108" s="9">
+        <v>2818</v>
+      </c>
+      <c r="P108" s="9">
+        <v>94</v>
+      </c>
+      <c r="Q108" s="9">
+        <v>1033</v>
+      </c>
+      <c r="R108" s="9">
+        <v>2715</v>
+      </c>
+      <c r="S108" s="9">
+        <v>1717</v>
+      </c>
     </row>
     <row r="109" spans="1:19">
       <c r="B109" s="4" t="s">
         <v>174</v>
       </c>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="O109">
+        <v>1054</v>
+      </c>
+      <c r="P109">
+        <v>143</v>
+      </c>
+      <c r="Q109">
+        <v>448</v>
+      </c>
+      <c r="R109">
+        <v>863</v>
+      </c>
+      <c r="S109">
+        <v>485</v>
+      </c>
     </row>
     <row r="111" spans="1:19">
       <c r="A111">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C111">
-        <v>50</v>
+        <v>373</v>
       </c>
       <c r="D111">
         <v>500</v>
@@ -4220,89 +5058,101 @@
         <v>20</v>
       </c>
       <c r="F111">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="G111" t="s">
-        <v>242</v>
+        <v>181</v>
       </c>
       <c r="H111" t="s">
-        <v>243</v>
-      </c>
-      <c r="I111" t="s">
-        <v>244</v>
-      </c>
-      <c r="J111" t="s">
-        <v>245</v>
-      </c>
-      <c r="K111" t="s">
-        <v>231</v>
+        <v>181</v>
       </c>
       <c r="M111">
-        <v>0</v>
-      </c>
-      <c r="O111">
-        <v>333</v>
-      </c>
-      <c r="P111">
-        <v>14</v>
-      </c>
-      <c r="Q111">
-        <v>253</v>
-      </c>
-      <c r="R111">
-        <v>314</v>
-      </c>
-      <c r="S111">
-        <v>73</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:19">
       <c r="A112" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="C112">
+        <v>373</v>
+      </c>
+      <c r="D112">
+        <v>500</v>
+      </c>
+      <c r="E112">
+        <v>20</v>
+      </c>
+      <c r="F112">
+        <v>200</v>
+      </c>
+      <c r="G112" t="s">
+        <v>181</v>
+      </c>
+      <c r="H112" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
       <c r="B113" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="C113">
+        <v>373</v>
+      </c>
+      <c r="D113">
+        <v>500</v>
+      </c>
+      <c r="E113">
+        <v>20</v>
+      </c>
+      <c r="F113">
+        <v>200</v>
+      </c>
+      <c r="G113" t="s">
+        <v>181</v>
+      </c>
+      <c r="H113" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
       <c r="B114" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:20">
       <c r="B115" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:20">
       <c r="B116" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:20">
       <c r="B117" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:20">
       <c r="B118" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:20">
       <c r="A120">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C120">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D120">
         <v>500</v>
@@ -4313,54 +5163,305 @@
       <c r="F120">
         <v>144</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H120" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="I120" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J120" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="K120" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="L120" s="9"/>
+      <c r="M120" s="9">
+        <v>0</v>
+      </c>
+      <c r="N120" s="9"/>
+      <c r="O120" s="9">
+        <v>296</v>
+      </c>
+      <c r="P120" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q120" s="9">
+        <v>220</v>
+      </c>
+      <c r="R120" s="9">
+        <v>287</v>
+      </c>
+      <c r="S120" s="9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
       <c r="A121" t="s">
         <v>204</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="G121" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H121" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="I121" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="J121" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="K121" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="L121" s="9"/>
+      <c r="M121" s="9">
+        <v>0</v>
+      </c>
+      <c r="N121" s="9"/>
+      <c r="O121" s="9">
+        <v>298</v>
+      </c>
+      <c r="P121" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q121" s="9">
+        <v>173</v>
+      </c>
+      <c r="R121" s="9">
+        <v>289</v>
+      </c>
+      <c r="S121" s="9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20">
       <c r="B122" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H122" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="I122" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="J122" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="K122" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="L122" s="9"/>
+      <c r="M122" s="9">
+        <v>0</v>
+      </c>
+      <c r="N122" s="9"/>
+      <c r="O122" s="9">
+        <v>251</v>
+      </c>
+      <c r="P122" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q122" s="9">
+        <v>180</v>
+      </c>
+      <c r="R122" s="9">
+        <v>245</v>
+      </c>
+      <c r="S122" s="9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20">
       <c r="B123" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="F123" s="12"/>
+      <c r="G123" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="H123" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="I123" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="J123" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="K123" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="L123" s="12"/>
+      <c r="M123" s="12">
+        <v>0</v>
+      </c>
+      <c r="O123" s="12">
+        <v>129</v>
+      </c>
+      <c r="P123" s="12">
+        <v>26</v>
+      </c>
+      <c r="Q123" s="12">
+        <v>61</v>
+      </c>
+      <c r="R123" s="12">
+        <v>96</v>
+      </c>
+      <c r="S123" s="12">
+        <v>45</v>
+      </c>
+      <c r="T123" s="12"/>
+    </row>
+    <row r="124" spans="1:20">
       <c r="B124" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
+      <c r="G124" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H124" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="I124" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="J124" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="K124" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="L124" s="12"/>
+      <c r="M124" s="12">
+        <v>0</v>
+      </c>
+      <c r="N124" s="12"/>
+      <c r="O124" s="12">
+        <v>171</v>
+      </c>
+      <c r="P124" s="12">
+        <v>8</v>
+      </c>
+      <c r="Q124" s="12">
+        <v>46</v>
+      </c>
+      <c r="R124" s="12">
+        <v>155</v>
+      </c>
+      <c r="S124" s="12">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20">
       <c r="B125" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="G125" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H125" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="I125" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="J125" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K125" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="L125" s="12"/>
+      <c r="M125" s="12">
+        <v>1</v>
+      </c>
+      <c r="O125" s="12">
+        <v>134</v>
+      </c>
+      <c r="P125" s="12">
+        <v>5</v>
+      </c>
+      <c r="Q125" s="12">
+        <v>66</v>
+      </c>
+      <c r="R125" s="12">
+        <v>104</v>
+      </c>
+      <c r="S125" s="12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20">
       <c r="B126" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="G126" s="9"/>
+      <c r="H126" s="9"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
+      <c r="L126" s="9"/>
+      <c r="M126" s="9"/>
+      <c r="N126" s="9"/>
+      <c r="O126" s="9">
+        <v>282</v>
+      </c>
+      <c r="P126" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q126" s="9">
+        <v>191</v>
+      </c>
+      <c r="R126" s="9">
+        <v>274</v>
+      </c>
+      <c r="S126" s="9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20">
       <c r="B127" s="4" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="O127" s="12">
+        <v>145</v>
+      </c>
+      <c r="P127" s="12">
+        <v>13</v>
+      </c>
+      <c r="Q127" s="12">
+        <v>58</v>
+      </c>
+      <c r="R127" s="12">
+        <v>118</v>
+      </c>
+      <c r="S127" s="12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19">
       <c r="A129">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C129">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D129">
         <v>500</v>
@@ -4371,43 +5472,893 @@
       <c r="F129">
         <v>144</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="G129" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H129" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="I129" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="J129" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="K129" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="L129" s="9"/>
+      <c r="M129" s="9">
+        <v>0</v>
+      </c>
+      <c r="N129" s="9"/>
+      <c r="O129" s="9">
+        <v>333</v>
+      </c>
+      <c r="P129" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q129" s="9">
+        <v>253</v>
+      </c>
+      <c r="R129" s="9">
+        <v>314</v>
+      </c>
+      <c r="S129" s="9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19">
       <c r="A130" t="s">
         <v>204</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="G130" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="H130" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="I130" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="J130" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="K130" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="L130" s="9"/>
+      <c r="M130" s="9">
+        <v>0</v>
+      </c>
+      <c r="N130" s="9"/>
+      <c r="O130" s="9">
+        <v>327</v>
+      </c>
+      <c r="P130" s="9">
+        <v>9</v>
+      </c>
+      <c r="Q130" s="9">
+        <v>238</v>
+      </c>
+      <c r="R130" s="9">
+        <v>314</v>
+      </c>
+      <c r="S130" s="9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19">
       <c r="B131" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="G131" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="H131" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="I131" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="J131" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="K131" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="L131" s="9"/>
+      <c r="M131" s="9">
+        <v>0</v>
+      </c>
+      <c r="N131" s="9"/>
+      <c r="O131" s="9">
+        <v>341</v>
+      </c>
+      <c r="P131" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q131" s="9">
+        <v>226</v>
+      </c>
+      <c r="R131" s="9">
+        <v>329</v>
+      </c>
+      <c r="S131" s="9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19">
       <c r="B132" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="G132" t="s">
+        <v>344</v>
+      </c>
+      <c r="H132" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="I132" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="J132" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="K132" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="L132" s="12"/>
+      <c r="M132" s="12">
+        <v>0</v>
+      </c>
+      <c r="O132" s="12">
+        <v>317</v>
+      </c>
+      <c r="P132" s="12">
+        <v>53</v>
+      </c>
+      <c r="Q132" s="12">
+        <v>201</v>
+      </c>
+      <c r="R132" s="12">
+        <v>150</v>
+      </c>
+      <c r="S132" s="12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19">
       <c r="B133" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="G133" t="s">
+        <v>349</v>
+      </c>
+      <c r="H133" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="I133" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J133" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="K133" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="L133" s="12"/>
+      <c r="M133" s="12">
+        <v>0</v>
+      </c>
+      <c r="O133" s="12">
+        <v>325</v>
+      </c>
+      <c r="P133" s="12">
+        <v>53</v>
+      </c>
+      <c r="Q133" s="12">
+        <v>112</v>
+      </c>
+      <c r="R133" s="12">
+        <v>253</v>
+      </c>
+      <c r="S133" s="12">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19">
       <c r="B134" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="G134" t="s">
+        <v>351</v>
+      </c>
+      <c r="H134" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="I134" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="J134" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="K134" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="L134" s="12"/>
+      <c r="M134" s="12">
+        <v>0</v>
+      </c>
+      <c r="O134" s="12">
+        <v>250</v>
+      </c>
+      <c r="P134" s="12">
+        <v>36</v>
+      </c>
+      <c r="Q134" s="12">
+        <v>88</v>
+      </c>
+      <c r="R134" s="12">
+        <v>195</v>
+      </c>
+      <c r="S134" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19">
       <c r="B135" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="9"/>
+      <c r="N135" s="9"/>
+      <c r="O135" s="9">
+        <v>334</v>
+      </c>
+      <c r="P135" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q135" s="9">
+        <v>239</v>
+      </c>
+      <c r="R135" s="9">
+        <v>319</v>
+      </c>
+      <c r="S135" s="9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19">
       <c r="B136" s="4" t="s">
         <v>174</v>
+      </c>
+      <c r="O136" s="12">
+        <v>297</v>
+      </c>
+      <c r="P136" s="12">
+        <v>47</v>
+      </c>
+      <c r="Q136" s="12">
+        <v>134</v>
+      </c>
+      <c r="R136" s="12">
+        <v>199</v>
+      </c>
+      <c r="S136" s="12">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19">
+      <c r="A138">
+        <v>14</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138">
+        <v>100</v>
+      </c>
+      <c r="D138">
+        <v>500</v>
+      </c>
+      <c r="E138">
+        <v>20</v>
+      </c>
+      <c r="F138">
+        <v>144</v>
+      </c>
+      <c r="G138" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="H138" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I138" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="J138" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="K138" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="L138" s="9"/>
+      <c r="M138" s="9">
+        <v>0</v>
+      </c>
+      <c r="N138" s="9"/>
+      <c r="O138" s="9">
+        <v>588</v>
+      </c>
+      <c r="P138" s="9">
+        <v>20</v>
+      </c>
+      <c r="Q138" s="9">
+        <v>438</v>
+      </c>
+      <c r="R138" s="9">
+        <v>566</v>
+      </c>
+      <c r="S138" s="9">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19">
+      <c r="A139" t="s">
+        <v>204</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G139" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="H139" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="I139" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="J139" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="K139" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="L139" s="9"/>
+      <c r="M139" s="9">
+        <v>0</v>
+      </c>
+      <c r="N139" s="9"/>
+      <c r="O139" s="9">
+        <v>675</v>
+      </c>
+      <c r="P139" s="9">
+        <v>17</v>
+      </c>
+      <c r="Q139" s="9">
+        <v>462</v>
+      </c>
+      <c r="R139" s="9">
+        <v>653</v>
+      </c>
+      <c r="S139" s="9">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19">
+      <c r="B140" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G140" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="H140" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="I140" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="J140" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="K140" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L140" s="9"/>
+      <c r="M140" s="9">
+        <v>1</v>
+      </c>
+      <c r="N140" s="9"/>
+      <c r="O140" s="9">
+        <v>527</v>
+      </c>
+      <c r="P140" s="9">
+        <v>35</v>
+      </c>
+      <c r="Q140" s="9">
+        <v>395</v>
+      </c>
+      <c r="R140" s="9">
+        <v>488</v>
+      </c>
+      <c r="S140" s="9">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19">
+      <c r="B141" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G141" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="H141" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="I141" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="J141" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="K141" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="M141" s="12">
+        <v>2</v>
+      </c>
+      <c r="O141" s="12">
+        <v>353</v>
+      </c>
+      <c r="P141" s="12">
+        <v>84</v>
+      </c>
+      <c r="Q141" s="12">
+        <v>140</v>
+      </c>
+      <c r="R141" s="12">
+        <v>259</v>
+      </c>
+      <c r="S141" s="12">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19">
+      <c r="B142" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G142" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="H142" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="I142" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="J142" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="K142" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="L142" s="12"/>
+      <c r="M142" s="12">
+        <v>2</v>
+      </c>
+      <c r="O142" s="12">
+        <v>308</v>
+      </c>
+      <c r="P142" s="12">
+        <v>49</v>
+      </c>
+      <c r="Q142" s="12">
+        <v>124</v>
+      </c>
+      <c r="R142" s="12">
+        <v>247</v>
+      </c>
+      <c r="S142" s="12">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19">
+      <c r="B143" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G143" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="H143" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="I143" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="J143" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="K143" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="L143" s="12"/>
+      <c r="M143" s="12">
+        <v>1</v>
+      </c>
+      <c r="O143" s="12">
+        <v>392</v>
+      </c>
+      <c r="P143" s="12">
+        <v>85</v>
+      </c>
+      <c r="Q143" s="12">
+        <v>162</v>
+      </c>
+      <c r="R143" s="12">
+        <v>367</v>
+      </c>
+      <c r="S143" s="12">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19">
+      <c r="B144" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G144" s="9"/>
+      <c r="H144" s="9"/>
+      <c r="I144" s="9"/>
+      <c r="J144" s="9"/>
+      <c r="K144" s="9"/>
+      <c r="L144" s="9"/>
+      <c r="M144" s="9"/>
+      <c r="N144" s="9"/>
+      <c r="O144" s="9">
+        <v>597</v>
+      </c>
+      <c r="P144" s="9">
+        <v>24</v>
+      </c>
+      <c r="Q144" s="9">
+        <v>432</v>
+      </c>
+      <c r="R144" s="9">
+        <v>569</v>
+      </c>
+      <c r="S144" s="9">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19">
+      <c r="B145" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O145" s="12">
+        <v>351</v>
+      </c>
+      <c r="P145" s="12">
+        <v>73</v>
+      </c>
+      <c r="Q145" s="12">
+        <v>142</v>
+      </c>
+      <c r="R145" s="12">
+        <v>291</v>
+      </c>
+      <c r="S145" s="12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19">
+      <c r="A147">
+        <v>15</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147">
+        <v>150</v>
+      </c>
+      <c r="D147">
+        <v>500</v>
+      </c>
+      <c r="E147">
+        <v>20</v>
+      </c>
+      <c r="F147">
+        <v>144</v>
+      </c>
+      <c r="G147" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="H147" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="I147" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="J147" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="K147" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="L147" s="9"/>
+      <c r="M147" s="9">
+        <v>0</v>
+      </c>
+      <c r="N147" s="9"/>
+      <c r="O147" s="9">
+        <v>809</v>
+      </c>
+      <c r="P147" s="9">
+        <v>48</v>
+      </c>
+      <c r="Q147" s="9">
+        <v>504</v>
+      </c>
+      <c r="R147" s="9">
+        <v>758</v>
+      </c>
+      <c r="S147" s="9">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19">
+      <c r="A148" t="s">
+        <v>204</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G148" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="H148" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="I148" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="J148" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="K148" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="L148" s="9"/>
+      <c r="M148" s="9">
+        <v>0</v>
+      </c>
+      <c r="N148" s="9"/>
+      <c r="O148" s="9">
+        <v>834</v>
+      </c>
+      <c r="P148" s="9">
+        <v>41</v>
+      </c>
+      <c r="Q148" s="9">
+        <v>525</v>
+      </c>
+      <c r="R148" s="9">
+        <v>787</v>
+      </c>
+      <c r="S148" s="9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19">
+      <c r="B149" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G149" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H149" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I149" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J149" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="K149" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="L149" s="9"/>
+      <c r="M149" s="9">
+        <v>0</v>
+      </c>
+      <c r="N149" s="9"/>
+      <c r="O149" s="9">
+        <v>767</v>
+      </c>
+      <c r="P149" s="9">
+        <v>47</v>
+      </c>
+      <c r="Q149" s="9">
+        <v>469</v>
+      </c>
+      <c r="R149" s="9">
+        <v>715</v>
+      </c>
+      <c r="S149" s="9">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19">
+      <c r="B150" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G150" t="s">
+        <v>319</v>
+      </c>
+      <c r="H150" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="I150" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="J150" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="K150" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="L150" s="12"/>
+      <c r="M150" s="12">
+        <v>0</v>
+      </c>
+      <c r="N150" s="12"/>
+      <c r="O150" s="12">
+        <v>393</v>
+      </c>
+      <c r="P150" s="12">
+        <v>51</v>
+      </c>
+      <c r="Q150" s="12">
+        <v>112</v>
+      </c>
+      <c r="R150" s="12">
+        <v>335</v>
+      </c>
+      <c r="S150" s="12">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19">
+      <c r="B151" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G151" t="s">
+        <v>324</v>
+      </c>
+      <c r="H151" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="I151" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="J151" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="K151" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="L151" s="13"/>
+      <c r="M151" s="13">
+        <v>2</v>
+      </c>
+      <c r="O151" s="12">
+        <v>500</v>
+      </c>
+      <c r="P151" s="12">
+        <v>49</v>
+      </c>
+      <c r="Q151" s="12">
+        <v>237</v>
+      </c>
+      <c r="R151" s="12">
+        <v>379</v>
+      </c>
+      <c r="S151" s="12">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19">
+      <c r="B152" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G152" t="s">
+        <v>328</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="I152" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="J152" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="K152" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="M152" s="12">
+        <v>1</v>
+      </c>
+      <c r="O152" s="12">
+        <v>492</v>
+      </c>
+      <c r="P152" s="12">
+        <v>60</v>
+      </c>
+      <c r="Q152" s="12">
+        <v>205</v>
+      </c>
+      <c r="R152" s="12">
+        <v>421</v>
+      </c>
+      <c r="S152" s="12">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19">
+      <c r="B153" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9"/>
+      <c r="L153" s="9"/>
+      <c r="M153" s="9"/>
+      <c r="N153" s="9"/>
+      <c r="O153" s="9">
+        <v>803</v>
+      </c>
+      <c r="P153" s="9">
+        <v>45</v>
+      </c>
+      <c r="Q153" s="9">
+        <v>499</v>
+      </c>
+      <c r="R153" s="9">
+        <v>753</v>
+      </c>
+      <c r="S153" s="9">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19">
+      <c r="B154" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="O154" s="12">
+        <v>462</v>
+      </c>
+      <c r="P154" s="12">
+        <v>53</v>
+      </c>
+      <c r="Q154" s="12">
+        <v>185</v>
+      </c>
+      <c r="R154" s="12">
+        <v>378</v>
+      </c>
+      <c r="S154" s="12">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New results, worked on 4.3
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="0" windowWidth="16720" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="17500" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="406">
   <si>
     <t>Testnummer</t>
   </si>
@@ -679,6 +679,9 @@
     <t>00:15:48h</t>
   </si>
   <si>
+    <t>a- Py</t>
+  </si>
+  <si>
     <t>01:08m</t>
   </si>
   <si>
@@ -1130,6 +1133,111 @@
   </si>
   <si>
     <t>00:37m</t>
+  </si>
+  <si>
+    <t>00:34:46h</t>
+  </si>
+  <si>
+    <t>29:04m</t>
+  </si>
+  <si>
+    <t>17:46m</t>
+  </si>
+  <si>
+    <t>05:05:54h</t>
+  </si>
+  <si>
+    <t>00:03:39h</t>
+  </si>
+  <si>
+    <t>05:03:17h</t>
+  </si>
+  <si>
+    <t>05:02:07h</t>
+  </si>
+  <si>
+    <t>15:11:08h</t>
+  </si>
+  <si>
+    <t>00:18:13h</t>
+  </si>
+  <si>
+    <t>01:23:17h</t>
+  </si>
+  <si>
+    <t>14:48:30h</t>
+  </si>
+  <si>
+    <t>13:40:10h</t>
+  </si>
+  <si>
+    <t>00:32:24h</t>
+  </si>
+  <si>
+    <t>01:59m</t>
+  </si>
+  <si>
+    <t>08:41m</t>
+  </si>
+  <si>
+    <t>26:58m</t>
+  </si>
+  <si>
+    <t>15:39m</t>
+  </si>
+  <si>
+    <t>00:32:18h</t>
+  </si>
+  <si>
+    <t>08:36m</t>
+  </si>
+  <si>
+    <t>26:35m</t>
+  </si>
+  <si>
+    <t>15:51m</t>
+  </si>
+  <si>
+    <t>00:58:10h</t>
+  </si>
+  <si>
+    <t>03:54m</t>
+  </si>
+  <si>
+    <t>16:07m</t>
+  </si>
+  <si>
+    <t>00:50:41h</t>
+  </si>
+  <si>
+    <t>00:34:10h</t>
+  </si>
+  <si>
+    <t>00:58:56h</t>
+  </si>
+  <si>
+    <t>03:42m</t>
+  </si>
+  <si>
+    <t>16:01m</t>
+  </si>
+  <si>
+    <t>00:51:42h</t>
+  </si>
+  <si>
+    <t>00:35:09h</t>
+  </si>
+  <si>
+    <t>01:00:28h</t>
+  </si>
+  <si>
+    <t>03:56m</t>
+  </si>
+  <si>
+    <t>00:52:53h</t>
+  </si>
+  <si>
+    <t>00:35:26h</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1305,106 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1266,7 +1472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="149">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1292,6 +1498,55 @@
     <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1317,6 +1572,55 @@
     <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1646,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T154"/>
+  <dimension ref="A1:T190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I106" workbookViewId="0">
-      <selection activeCell="S128" sqref="S128"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3530,21 +3834,41 @@
       <c r="F49">
         <v>144</v>
       </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
+      <c r="G49" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="L49" s="9"/>
       <c r="M49" s="9">
         <v>1</v>
       </c>
       <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
+      <c r="O49" s="9">
+        <v>18354</v>
+      </c>
+      <c r="P49" s="9">
+        <v>150</v>
+      </c>
+      <c r="Q49" s="9">
+        <v>219</v>
+      </c>
+      <c r="R49" s="9">
+        <v>18197</v>
+      </c>
+      <c r="S49" s="9">
+        <v>18127</v>
+      </c>
     </row>
     <row r="50" spans="1:19">
       <c r="B50" s="4" t="s">
@@ -3582,11 +3906,23 @@
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
-      <c r="Q53" s="9"/>
-      <c r="R53" s="9"/>
-      <c r="S53" s="9"/>
+      <c r="O53" s="9">
+        <f>AVERAGE(O47:O49)</f>
+        <v>20343</v>
+      </c>
+      <c r="P53" s="9">
+        <f>AVERAGE(P47:P49)</f>
+        <v>132</v>
+      </c>
+      <c r="Q53" s="9">
+        <v>246</v>
+      </c>
+      <c r="R53" s="9">
+        <v>20205</v>
+      </c>
+      <c r="S53" s="9">
+        <v>20089</v>
+      </c>
     </row>
     <row r="54" spans="1:19">
       <c r="B54" s="4" t="s">
@@ -3736,7 +4072,7 @@
         <v>116</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="L58" s="9" t="s">
         <v>103</v>
@@ -3809,16 +4145,16 @@
         <v>144</v>
       </c>
       <c r="G61" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="J61" s="9" t="s">
         <v>222</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="I61" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="J61" s="9" t="s">
-        <v>221</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>215</v>
@@ -3864,19 +4200,19 @@
         <v>144</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J62" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K62" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L62" s="9"/>
       <c r="M62" s="9">
@@ -3916,19 +4252,19 @@
         <v>144</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>126</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K63" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L63" s="9"/>
       <c r="M63" s="9">
@@ -4076,20 +4412,20 @@
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="2">
-        <v>0.63273148148148151</v>
-      </c>
-      <c r="H69" s="2">
-        <v>1.2650462962962962E-2</v>
-      </c>
-      <c r="I69" s="2">
-        <v>5.783564814814815E-2</v>
-      </c>
-      <c r="J69" s="2">
-        <v>0.61701388888888886</v>
-      </c>
-      <c r="K69" s="2">
-        <v>0.56956018518518514</v>
+      <c r="G69" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="K69" s="2" t="s">
+        <v>382</v>
       </c>
       <c r="M69" s="5">
         <v>0</v>
@@ -4160,7 +4496,7 @@
     </row>
     <row r="75" spans="1:19">
       <c r="A75" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>12</v>
@@ -4208,36 +4544,126 @@
     </row>
     <row r="78" spans="1:19">
       <c r="B78" s="4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
+      <c r="G78" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>3490</v>
+      </c>
+      <c r="P78">
+        <v>234</v>
+      </c>
+      <c r="Q78">
+        <v>967</v>
+      </c>
+      <c r="R78">
+        <v>3041</v>
+      </c>
+      <c r="S78">
+        <v>2050</v>
+      </c>
     </row>
     <row r="79" spans="1:19">
       <c r="B79" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="G79" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="K79" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>3536</v>
+      </c>
+      <c r="P79">
+        <v>222</v>
+      </c>
+      <c r="Q79">
+        <v>961</v>
+      </c>
+      <c r="R79">
+        <v>3102</v>
+      </c>
+      <c r="S79">
+        <v>2109</v>
+      </c>
     </row>
     <row r="80" spans="1:19">
       <c r="B80" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
+      <c r="G80" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+      <c r="O80">
+        <v>3628</v>
+      </c>
+      <c r="P80">
+        <v>236</v>
+      </c>
+      <c r="Q80">
+        <v>996</v>
+      </c>
+      <c r="R80">
+        <v>3173</v>
+      </c>
+      <c r="S80">
+        <v>2126</v>
+      </c>
     </row>
     <row r="81" spans="1:19">
       <c r="B81" s="4" t="s">
@@ -4260,6 +4686,21 @@
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
+      <c r="O82">
+        <v>3551</v>
+      </c>
+      <c r="P82">
+        <v>231</v>
+      </c>
+      <c r="Q82">
+        <v>975</v>
+      </c>
+      <c r="R82">
+        <v>3105</v>
+      </c>
+      <c r="S82">
+        <v>2095</v>
+      </c>
     </row>
     <row r="83" spans="1:19">
       <c r="B83" s="4"/>
@@ -4272,7 +4713,7 @@
     </row>
     <row r="84" spans="1:19">
       <c r="A84" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>12</v>
@@ -4320,36 +4761,126 @@
     </row>
     <row r="87" spans="1:19">
       <c r="B87" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
+      <c r="G87" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>2086</v>
+      </c>
+      <c r="P87">
+        <v>126</v>
+      </c>
+      <c r="Q87">
+        <v>525</v>
+      </c>
+      <c r="R87">
+        <v>1744</v>
+      </c>
+      <c r="S87">
+        <v>1066</v>
+      </c>
     </row>
     <row r="88" spans="1:19">
       <c r="B88" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
+      <c r="G88" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+      <c r="O88">
+        <v>1944</v>
+      </c>
+      <c r="P88">
+        <v>119</v>
+      </c>
+      <c r="Q88">
+        <v>521</v>
+      </c>
+      <c r="R88">
+        <v>1618</v>
+      </c>
+      <c r="S88">
+        <v>939</v>
+      </c>
     </row>
     <row r="89" spans="1:19">
       <c r="B89" s="4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
+      <c r="G89" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>1938</v>
+      </c>
+      <c r="P89">
+        <v>131</v>
+      </c>
+      <c r="Q89">
+        <v>516</v>
+      </c>
+      <c r="R89">
+        <v>1595</v>
+      </c>
+      <c r="S89">
+        <v>951</v>
+      </c>
     </row>
     <row r="90" spans="1:19">
       <c r="B90" s="4" t="s">
@@ -4361,6 +4892,21 @@
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
+      <c r="O90">
+        <v>1989</v>
+      </c>
+      <c r="P90">
+        <v>125</v>
+      </c>
+      <c r="Q90">
+        <v>521</v>
+      </c>
+      <c r="R90">
+        <v>1652</v>
+      </c>
+      <c r="S90">
+        <v>985</v>
+      </c>
     </row>
     <row r="91" spans="1:19">
       <c r="B91" s="4" t="s">
@@ -4383,7 +4929,7 @@
     </row>
     <row r="93" spans="1:19">
       <c r="A93" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>12</v>
@@ -4401,19 +4947,19 @@
         <v>50</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I93" s="11" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="J93" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="K93" s="11" t="s">
         <v>303</v>
-      </c>
-      <c r="K93" s="11" t="s">
-        <v>302</v>
       </c>
       <c r="L93" s="9"/>
       <c r="M93" s="9">
@@ -4456,30 +5002,40 @@
         <v>50</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="J94" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L94" s="9"/>
       <c r="M94" s="9">
         <v>0</v>
       </c>
       <c r="N94" s="9"/>
-      <c r="O94" s="9"/>
-      <c r="P94" s="9"/>
-      <c r="Q94" s="9"/>
-      <c r="R94" s="9"/>
-      <c r="S94" s="9"/>
+      <c r="O94" s="9">
+        <v>3779</v>
+      </c>
+      <c r="P94" s="9">
+        <v>86</v>
+      </c>
+      <c r="Q94" s="9">
+        <v>976</v>
+      </c>
+      <c r="R94" s="9">
+        <v>3686</v>
+      </c>
+      <c r="S94" s="9">
+        <v>2759</v>
+      </c>
     </row>
     <row r="95" spans="1:19">
       <c r="B95" s="4" t="s">
@@ -4498,30 +5054,40 @@
         <v>50</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="L95" s="9"/>
       <c r="M95" s="9">
         <v>0</v>
       </c>
       <c r="N95" s="9"/>
-      <c r="O95" s="9"/>
-      <c r="P95" s="9"/>
-      <c r="Q95" s="9"/>
-      <c r="R95" s="9"/>
-      <c r="S95" s="9"/>
+      <c r="O95" s="9">
+        <v>3799</v>
+      </c>
+      <c r="P95" s="9">
+        <v>87</v>
+      </c>
+      <c r="Q95" s="9">
+        <v>996</v>
+      </c>
+      <c r="R95" s="9">
+        <v>3705</v>
+      </c>
+      <c r="S95" s="9">
+        <v>2737</v>
+      </c>
     </row>
     <row r="96" spans="1:19">
       <c r="B96" s="4" t="s">
@@ -4667,11 +5233,21 @@
       <c r="L99" s="9"/>
       <c r="M99" s="9"/>
       <c r="N99" s="9"/>
-      <c r="O99" s="9"/>
-      <c r="P99" s="9"/>
-      <c r="Q99" s="9"/>
-      <c r="R99" s="9"/>
-      <c r="S99" s="9"/>
+      <c r="O99" s="9">
+        <v>3840</v>
+      </c>
+      <c r="P99" s="9">
+        <v>87</v>
+      </c>
+      <c r="Q99" s="9">
+        <v>1034</v>
+      </c>
+      <c r="R99" s="9">
+        <v>3746</v>
+      </c>
+      <c r="S99" s="9">
+        <v>2754</v>
+      </c>
     </row>
     <row r="100" spans="1:19">
       <c r="B100" s="4" t="s">
@@ -4727,19 +5303,19 @@
         <v>100</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H102" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I102" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J102" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K102" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L102" s="9"/>
       <c r="M102" s="9">
@@ -4782,19 +5358,19 @@
         <v>100</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H103" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="I103" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K103" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L103" s="9"/>
       <c r="M103" s="9">
@@ -4834,19 +5410,19 @@
         <v>100</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H104" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K104" s="9" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L104" s="9"/>
       <c r="M104" s="9">
@@ -5164,19 +5740,19 @@
         <v>144</v>
       </c>
       <c r="G120" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H120" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I120" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J120" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="K120" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L120" s="9"/>
       <c r="M120" s="9">
@@ -5207,19 +5783,19 @@
         <v>13</v>
       </c>
       <c r="G121" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H121" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I121" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J121" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="K121" s="9" t="s">
         <v>236</v>
-      </c>
-      <c r="K121" s="9" t="s">
-        <v>235</v>
       </c>
       <c r="L121" s="9"/>
       <c r="M121" s="9">
@@ -5247,19 +5823,19 @@
         <v>14</v>
       </c>
       <c r="G122" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H122" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I122" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J122" s="9" t="s">
         <v>108</v>
       </c>
       <c r="K122" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L122" s="9"/>
       <c r="M122" s="9">
@@ -5288,19 +5864,19 @@
       </c>
       <c r="F123" s="12"/>
       <c r="G123" s="12" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H123" s="12" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I123" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J123" s="12" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="K123" s="12" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="L123" s="12"/>
       <c r="M123" s="12">
@@ -5331,19 +5907,19 @@
       <c r="E124" s="12"/>
       <c r="F124" s="12"/>
       <c r="G124" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H124" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I124" s="12" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="J124" s="12" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K124" s="12" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L124" s="12"/>
       <c r="M124" s="12">
@@ -5374,16 +5950,16 @@
         <v>92</v>
       </c>
       <c r="H125" s="12" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="I125" s="12" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="J125" s="12" t="s">
         <v>54</v>
       </c>
       <c r="K125" s="12" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L125" s="12"/>
       <c r="M125" s="12">
@@ -5473,19 +6049,19 @@
         <v>144</v>
       </c>
       <c r="G129" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H129" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="I129" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J129" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="K129" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L129" s="9"/>
       <c r="M129" s="9">
@@ -5516,19 +6092,19 @@
         <v>13</v>
       </c>
       <c r="G130" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H130" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="I130" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="J130" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="H130" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="I130" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="J130" s="9" t="s">
-        <v>246</v>
-      </c>
       <c r="K130" s="9" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L130" s="9"/>
       <c r="M130" s="9">
@@ -5556,19 +6132,19 @@
         <v>14</v>
       </c>
       <c r="G131" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H131" s="9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I131" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="J131" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="K131" s="9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L131" s="9"/>
       <c r="M131" s="9">
@@ -5596,19 +6172,19 @@
         <v>117</v>
       </c>
       <c r="G132" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H132" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I132" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J132" s="12" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="K132" s="12" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L132" s="12"/>
       <c r="M132" s="12">
@@ -5635,19 +6211,19 @@
         <v>123</v>
       </c>
       <c r="G133" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H133" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I133" s="12" t="s">
         <v>100</v>
       </c>
       <c r="J133" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="K133" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="L133" s="12"/>
       <c r="M133" s="12">
@@ -5674,19 +6250,19 @@
         <v>124</v>
       </c>
       <c r="G134" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="H134" s="12" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="I134" s="12" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="J134" s="12" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="K134" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L134" s="12"/>
       <c r="M134" s="12">
@@ -5776,19 +6352,19 @@
         <v>144</v>
       </c>
       <c r="G138" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H138" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="J138" s="9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="K138" s="9" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L138" s="9"/>
       <c r="M138" s="9">
@@ -5819,19 +6395,19 @@
         <v>13</v>
       </c>
       <c r="G139" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H139" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J139" s="9" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K139" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L139" s="9"/>
       <c r="M139" s="9">
@@ -5859,19 +6435,19 @@
         <v>14</v>
       </c>
       <c r="G140" s="9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H140" s="9" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I140" s="9" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J140" s="9" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K140" s="9" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="L140" s="9"/>
       <c r="M140" s="9">
@@ -5899,19 +6475,19 @@
         <v>117</v>
       </c>
       <c r="G141" s="12" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H141" s="12" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="I141" s="12" t="s">
         <v>146</v>
       </c>
       <c r="J141" s="12" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="K141" s="12" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="M141" s="12">
         <v>2</v>
@@ -5937,19 +6513,19 @@
         <v>123</v>
       </c>
       <c r="G142" s="12" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H142" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I142" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J142" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K142" s="12" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L142" s="12"/>
       <c r="M142" s="12">
@@ -5976,19 +6552,19 @@
         <v>124</v>
       </c>
       <c r="G143" s="12" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H143" s="12" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I143" s="12" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="J143" s="12" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K143" s="12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="L143" s="12"/>
       <c r="M143" s="12">
@@ -6078,19 +6654,19 @@
         <v>144</v>
       </c>
       <c r="G147" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="H147" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="I147" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J147" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="H147" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="I147" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="J147" s="9" t="s">
-        <v>273</v>
-      </c>
       <c r="K147" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L147" s="9"/>
       <c r="M147" s="9">
@@ -6121,19 +6697,19 @@
         <v>13</v>
       </c>
       <c r="G148" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H148" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I148" s="9" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="J148" s="9" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="K148" s="9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L148" s="9"/>
       <c r="M148" s="9">
@@ -6161,19 +6737,19 @@
         <v>14</v>
       </c>
       <c r="G149" s="9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H149" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I149" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="J149" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="K149" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="L149" s="9"/>
       <c r="M149" s="9">
@@ -6201,19 +6777,19 @@
         <v>117</v>
       </c>
       <c r="G150" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H150" s="12" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I150" s="12" t="s">
         <v>100</v>
       </c>
       <c r="J150" s="12" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="K150" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="L150" s="12"/>
       <c r="M150" s="12">
@@ -6241,19 +6817,19 @@
         <v>123</v>
       </c>
       <c r="G151" t="s">
+        <v>325</v>
+      </c>
+      <c r="H151" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="H151" s="13" t="s">
-        <v>323</v>
-      </c>
       <c r="I151" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="J151" s="13" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="K151" s="13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="L151" s="13"/>
       <c r="M151" s="13">
@@ -6280,19 +6856,19 @@
         <v>124</v>
       </c>
       <c r="G152" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I152" s="12" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="J152" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K152" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M152" s="12">
         <v>1</v>
@@ -6360,6 +6936,261 @@
       <c r="S154" s="12">
         <v>163</v>
       </c>
+    </row>
+    <row r="156" spans="1:19">
+      <c r="A156">
+        <v>16</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C156">
+        <v>150</v>
+      </c>
+      <c r="D156">
+        <v>50</v>
+      </c>
+      <c r="E156">
+        <v>10</v>
+      </c>
+      <c r="F156">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19">
+      <c r="B157" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19">
+      <c r="B158" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19">
+      <c r="B159" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19">
+      <c r="B160" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="B161" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="B162" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="B163" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165">
+        <v>17</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C165">
+        <v>150</v>
+      </c>
+      <c r="D165">
+        <v>100</v>
+      </c>
+      <c r="E165">
+        <v>10</v>
+      </c>
+      <c r="F165">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="B166" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="B167" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="B168" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="B169" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="B170" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="B171" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="B172" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174">
+        <v>18</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C174">
+        <v>150</v>
+      </c>
+      <c r="D174">
+        <v>200</v>
+      </c>
+      <c r="E174">
+        <v>20</v>
+      </c>
+      <c r="F174">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="B175" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="B176" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="B177" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="B178" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="B179" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="B180" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="B181" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="4">
+        <v>16</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C183" s="4">
+        <v>150</v>
+      </c>
+      <c r="D183" s="4">
+        <v>400</v>
+      </c>
+      <c r="E183" s="4">
+        <v>20</v>
+      </c>
+      <c r="F183" s="4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="4"/>
+      <c r="B184" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C184" s="4"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="4"/>
+      <c r="B185" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C185" s="4"/>
+      <c r="D185" s="4"/>
+      <c r="E185" s="4"/>
+      <c r="F185" s="4"/>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="4"/>
+      <c r="B186" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C186" s="4"/>
+      <c r="D186" s="4"/>
+      <c r="E186" s="4"/>
+      <c r="F186" s="4"/>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="4"/>
+      <c r="B187" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C187" s="4"/>
+      <c r="D187" s="4"/>
+      <c r="E187" s="4"/>
+      <c r="F187" s="4"/>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="4"/>
+      <c r="B188" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C188" s="4"/>
+      <c r="D188" s="4"/>
+      <c r="E188" s="4"/>
+      <c r="F188" s="4"/>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="4"/>
+      <c r="B189" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C189" s="4"/>
+      <c r="D189" s="4"/>
+      <c r="E189" s="4"/>
+      <c r="F189" s="4"/>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="4"/>
+      <c r="B190" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C190" s="4"/>
+      <c r="D190" s="4"/>
+      <c r="E190" s="4"/>
+      <c r="F190" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6377,7 +7208,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Almost finished. Updated results.
</commit_message>
<xml_diff>
--- a/Code/Results.xlsx
+++ b/Code/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="17500" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="14620" yWindow="0" windowWidth="20740" windowHeight="15960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="482">
   <si>
     <t>Testnummer</t>
   </si>
@@ -1238,6 +1238,234 @@
   </si>
   <si>
     <t>00:35:26h</t>
+  </si>
+  <si>
+    <t>05:49:49h</t>
+  </si>
+  <si>
+    <t>02:12m</t>
+  </si>
+  <si>
+    <t>24:40m</t>
+  </si>
+  <si>
+    <t>05:47:29h</t>
+  </si>
+  <si>
+    <t>05:24:17h</t>
+  </si>
+  <si>
+    <t>03:03:27h</t>
+  </si>
+  <si>
+    <t>02:32m</t>
+  </si>
+  <si>
+    <t>03:00:49h</t>
+  </si>
+  <si>
+    <t>22:38m</t>
+  </si>
+  <si>
+    <t>02:40:12h</t>
+  </si>
+  <si>
+    <t>03:01:50h</t>
+  </si>
+  <si>
+    <t>23:45m</t>
+  </si>
+  <si>
+    <t>03:00:10h</t>
+  </si>
+  <si>
+    <t>02:37:26h</t>
+  </si>
+  <si>
+    <t>07:39m</t>
+  </si>
+  <si>
+    <t>00:43m</t>
+  </si>
+  <si>
+    <t>04:14m</t>
+  </si>
+  <si>
+    <t>06:49m</t>
+  </si>
+  <si>
+    <t>03:12m</t>
+  </si>
+  <si>
+    <t>00:42m</t>
+  </si>
+  <si>
+    <t>07:04m</t>
+  </si>
+  <si>
+    <t>02:41m</t>
+  </si>
+  <si>
+    <t>08:38m</t>
+  </si>
+  <si>
+    <t>00:59m</t>
+  </si>
+  <si>
+    <t>05:44m</t>
+  </si>
+  <si>
+    <t>07:26m</t>
+  </si>
+  <si>
+    <t>02:37m</t>
+  </si>
+  <si>
+    <t>02:18m</t>
+  </si>
+  <si>
+    <t>00:30m</t>
+  </si>
+  <si>
+    <t>00:50m</t>
+  </si>
+  <si>
+    <t>01:33m</t>
+  </si>
+  <si>
+    <t>01:15m</t>
+  </si>
+  <si>
+    <t>03:30m</t>
+  </si>
+  <si>
+    <t>02:15m</t>
+  </si>
+  <si>
+    <t>02:44m</t>
+  </si>
+  <si>
+    <t>01:09m</t>
+  </si>
+  <si>
+    <t>00:32m</t>
+  </si>
+  <si>
+    <t>01:30m</t>
+  </si>
+  <si>
+    <t>02:05m</t>
+  </si>
+  <si>
+    <t>01:18m</t>
+  </si>
+  <si>
+    <t>00:56m</t>
+  </si>
+  <si>
+    <t>00:16m</t>
+  </si>
+  <si>
+    <t>02:02m</t>
+  </si>
+  <si>
+    <t>00:29m</t>
+  </si>
+  <si>
+    <t>00:57m</t>
+  </si>
+  <si>
+    <t>00:44m</t>
+  </si>
+  <si>
+    <t>00:22m</t>
+  </si>
+  <si>
+    <t>01:51m</t>
+  </si>
+  <si>
+    <t>01:14m</t>
+  </si>
+  <si>
+    <t>06:40m</t>
+  </si>
+  <si>
+    <t>05:40m</t>
+  </si>
+  <si>
+    <t>03:47m</t>
+  </si>
+  <si>
+    <t>05:37m</t>
+  </si>
+  <si>
+    <t>06:25m</t>
+  </si>
+  <si>
+    <t>00:55m</t>
+  </si>
+  <si>
+    <t>02:58m</t>
+  </si>
+  <si>
+    <t>04:01m</t>
+  </si>
+  <si>
+    <t>03:14m</t>
+  </si>
+  <si>
+    <t>02:17m</t>
+  </si>
+  <si>
+    <t>03:36m</t>
+  </si>
+  <si>
+    <t>01:04m</t>
+  </si>
+  <si>
+    <t>02:13m</t>
+  </si>
+  <si>
+    <t>00:40m</t>
+  </si>
+  <si>
+    <t>00:39m</t>
+  </si>
+  <si>
+    <t>00:28m</t>
+  </si>
+  <si>
+    <t>00:25m</t>
+  </si>
+  <si>
+    <t>01:16m</t>
+  </si>
+  <si>
+    <t>03:05m</t>
+  </si>
+  <si>
+    <t>00:31m</t>
+  </si>
+  <si>
+    <t>02:21m</t>
+  </si>
+  <si>
+    <t>Gesamt</t>
+  </si>
+  <si>
+    <t>Cut</t>
+  </si>
+  <si>
+    <t>Analyze</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>OBSOLETE</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1295,6 +1523,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1305,7 +1539,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="149">
+  <cellStyleXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1455,8 +1689,170 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1471,8 +1867,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="149">
+  <cellStyles count="311">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1547,6 +1944,87 @@
     <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="310" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1621,6 +2099,87 @@
     <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="309" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1950,19 +2509,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T190"/>
+  <dimension ref="A1:Z190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" customWidth="1"/>
     <col min="6" max="6" width="5.1640625" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
@@ -2512,6 +3071,9 @@
       </c>
     </row>
     <row r="13" spans="1:19">
+      <c r="A13" s="14" t="s">
+        <v>201</v>
+      </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -2562,7 +3124,7 @@
         <v>2808</v>
       </c>
       <c r="S13" s="9">
-        <v>1227</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2749,7 +3311,7 @@
         <v>2716</v>
       </c>
       <c r="S17" s="9">
-        <v>1522</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -3818,7 +4380,7 @@
         <v>21123</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:26">
       <c r="B49" t="s">
         <v>14</v>
       </c>
@@ -3870,7 +4432,7 @@
         <v>18127</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:26">
       <c r="B50" s="4" t="s">
         <v>117</v>
       </c>
@@ -3878,7 +4440,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:26">
       <c r="B51" s="4" t="s">
         <v>123</v>
       </c>
@@ -3886,7 +4448,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:26">
       <c r="B52" s="4" t="s">
         <v>124</v>
       </c>
@@ -3894,7 +4456,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:26">
       <c r="B53" s="4" t="s">
         <v>173</v>
       </c>
@@ -3924,12 +4486,32 @@
         <v>20089</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:26">
       <c r="B54" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="55" spans="1:26">
+      <c r="U55" t="s">
+        <v>476</v>
+      </c>
+      <c r="V55" t="s">
+        <v>182</v>
+      </c>
+      <c r="W55" t="s">
+        <v>477</v>
+      </c>
+      <c r="X55" t="s">
+        <v>478</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>479</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26">
       <c r="A56">
         <v>7</v>
       </c>
@@ -3986,7 +4568,7 @@
         <v>6051</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:26">
       <c r="A57" t="s">
         <v>203</v>
       </c>
@@ -4043,7 +4625,7 @@
         <v>6492</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:26">
       <c r="B58" t="s">
         <v>14</v>
       </c>
@@ -4097,7 +4679,7 @@
         <v>5945</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:26">
       <c r="B59" s="4" t="s">
         <v>157</v>
       </c>
@@ -4125,7 +4707,7 @@
         <v>6163</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:26">
       <c r="A61">
         <v>8</v>
       </c>
@@ -4179,8 +4761,11 @@
       <c r="S61" s="9">
         <v>966</v>
       </c>
-    </row>
-    <row r="62" spans="1:19">
+      <c r="Z61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26">
       <c r="A62" t="s">
         <v>203</v>
       </c>
@@ -4235,7 +4820,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:26">
       <c r="B63" s="4" t="s">
         <v>14</v>
       </c>
@@ -4287,7 +4872,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:26">
       <c r="B64" s="4" t="s">
         <v>173</v>
       </c>
@@ -4361,7 +4946,7 @@
       <c r="S66" s="9"/>
     </row>
     <row r="67" spans="1:19">
-      <c r="A67" t="s">
+      <c r="A67" s="14" t="s">
         <v>201</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -4495,7 +5080,7 @@
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:19">
-      <c r="A75" t="s">
+      <c r="A75" s="14" t="s">
         <v>362</v>
       </c>
       <c r="B75" s="4" t="s">
@@ -4712,7 +5297,7 @@
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="1:19">
-      <c r="A84" t="s">
+      <c r="A84" s="14" t="s">
         <v>361</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -4730,9 +5315,41 @@
       <c r="F84" s="5">
         <v>12</v>
       </c>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
+      <c r="G84" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="H84" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="I84" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="J84" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="K84" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9">
+        <v>0</v>
+      </c>
+      <c r="N84" s="9"/>
+      <c r="O84" s="9">
+        <v>20989</v>
+      </c>
+      <c r="P84" s="9">
+        <v>132</v>
+      </c>
+      <c r="Q84" s="9">
+        <v>1480</v>
+      </c>
+      <c r="R84" s="9">
+        <v>20849</v>
+      </c>
+      <c r="S84" s="9">
+        <v>19457</v>
+      </c>
     </row>
     <row r="85" spans="1:19">
       <c r="A85" t="s">
@@ -4744,9 +5361,41 @@
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
+      <c r="G85" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="I85" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="J85" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="K85" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9">
+        <v>0</v>
+      </c>
+      <c r="N85" s="9"/>
+      <c r="O85" s="9">
+        <v>11007</v>
+      </c>
+      <c r="P85" s="9">
+        <v>152</v>
+      </c>
+      <c r="Q85" s="9">
+        <v>1358</v>
+      </c>
+      <c r="R85" s="9">
+        <v>10849</v>
+      </c>
+      <c r="S85" s="9">
+        <v>9612</v>
+      </c>
     </row>
     <row r="86" spans="1:19">
       <c r="B86" s="4" t="s">
@@ -4755,9 +5404,41 @@
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
+      <c r="G86" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="H86" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I86" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="J86" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="K86" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="L86" s="9"/>
+      <c r="M86" s="9">
+        <v>0</v>
+      </c>
+      <c r="N86" s="9"/>
+      <c r="O86" s="9">
+        <v>10910</v>
+      </c>
+      <c r="P86" s="9">
+        <v>103</v>
+      </c>
+      <c r="Q86" s="9">
+        <v>1425</v>
+      </c>
+      <c r="R86" s="9">
+        <v>10810</v>
+      </c>
+      <c r="S86" s="9">
+        <v>9446</v>
+      </c>
     </row>
     <row r="87" spans="1:19">
       <c r="B87" s="4" t="s">
@@ -4889,23 +5570,31 @@
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="O90">
-        <v>1989</v>
-      </c>
-      <c r="P90">
-        <v>125</v>
-      </c>
-      <c r="Q90">
-        <v>521</v>
-      </c>
-      <c r="R90">
-        <v>1652</v>
-      </c>
-      <c r="S90">
-        <v>985</v>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="9">
+        <f>AVERAGE(O84:O86)</f>
+        <v>14302</v>
+      </c>
+      <c r="P90" s="9">
+        <f>AVERAGE(P84:P86)</f>
+        <v>129</v>
+      </c>
+      <c r="Q90" s="9">
+        <f>AVERAGE(Q84:Q86)</f>
+        <v>1421</v>
+      </c>
+      <c r="R90" s="9">
+        <v>14169</v>
+      </c>
+      <c r="S90" s="9">
+        <v>12838</v>
       </c>
     </row>
     <row r="91" spans="1:19">
@@ -4918,6 +5607,21 @@
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
+      <c r="O91">
+        <v>1989</v>
+      </c>
+      <c r="P91">
+        <v>125</v>
+      </c>
+      <c r="Q91">
+        <v>521</v>
+      </c>
+      <c r="R91">
+        <v>1652</v>
+      </c>
+      <c r="S91">
+        <v>985</v>
+      </c>
     </row>
     <row r="92" spans="1:19">
       <c r="D92" s="5"/>
@@ -4928,7 +5632,7 @@
       <c r="I92" s="5"/>
     </row>
     <row r="93" spans="1:19">
-      <c r="A93" t="s">
+      <c r="A93" s="14" t="s">
         <v>367</v>
       </c>
       <c r="B93" s="4" t="s">
@@ -5284,7 +5988,7 @@
       <c r="I101" s="5"/>
     </row>
     <row r="102" spans="1:19">
-      <c r="A102">
+      <c r="A102" s="14">
         <v>10</v>
       </c>
       <c r="B102" s="4" t="s">
@@ -5556,7 +6260,7 @@
         <v>215</v>
       </c>
       <c r="Q107">
-        <v>705</v>
+        <v>405</v>
       </c>
       <c r="R107">
         <v>830</v>
@@ -5608,7 +6312,7 @@
         <v>143</v>
       </c>
       <c r="Q109">
-        <v>448</v>
+        <v>348</v>
       </c>
       <c r="R109">
         <v>863</v>
@@ -5618,7 +6322,7 @@
       </c>
     </row>
     <row r="111" spans="1:19">
-      <c r="A111">
+      <c r="A111" s="14">
         <v>11</v>
       </c>
       <c r="B111" s="4" t="s">
@@ -5721,7 +6425,7 @@
       </c>
     </row>
     <row r="120" spans="1:20">
-      <c r="A120">
+      <c r="A120" s="14">
         <v>12</v>
       </c>
       <c r="B120" s="4" t="s">
@@ -6030,7 +6734,7 @@
       </c>
     </row>
     <row r="129" spans="1:19">
-      <c r="A129">
+      <c r="A129" s="14">
         <v>13</v>
       </c>
       <c r="B129" s="4" t="s">
@@ -6333,7 +7037,7 @@
       </c>
     </row>
     <row r="138" spans="1:19">
-      <c r="A138">
+      <c r="A138" s="14">
         <v>14</v>
       </c>
       <c r="B138" s="4" t="s">
@@ -6635,7 +7339,7 @@
       </c>
     </row>
     <row r="147" spans="1:19">
-      <c r="A147">
+      <c r="A147" s="14">
         <v>15</v>
       </c>
       <c r="B147" s="4" t="s">
@@ -6956,43 +7660,294 @@
       <c r="F156">
         <v>144</v>
       </c>
+      <c r="G156" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="H156" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="I156" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="J156" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="K156" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="L156" s="9"/>
+      <c r="M156" s="9">
+        <v>0</v>
+      </c>
+      <c r="N156" s="9"/>
+      <c r="O156" s="9">
+        <v>84</v>
+      </c>
+      <c r="P156" s="9">
+        <v>26</v>
+      </c>
+      <c r="Q156" s="9">
+        <v>44</v>
+      </c>
+      <c r="R156" s="9">
+        <v>44</v>
+      </c>
+      <c r="S156" s="9">
+        <v>22</v>
+      </c>
     </row>
     <row r="157" spans="1:19">
+      <c r="A157" t="s">
+        <v>203</v>
+      </c>
       <c r="B157" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="G157" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="H157" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="I157" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="J157" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="K157" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="L157" s="9"/>
+      <c r="M157" s="9">
+        <v>0</v>
+      </c>
+      <c r="N157" s="9"/>
+      <c r="O157" s="9">
+        <v>75</v>
+      </c>
+      <c r="P157" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q157" s="9">
+        <v>46</v>
+      </c>
+      <c r="R157" s="9">
+        <v>41</v>
+      </c>
+      <c r="S157" s="9">
+        <v>22</v>
       </c>
     </row>
     <row r="158" spans="1:19">
       <c r="B158" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="G158" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="H158" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="I158" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="J158" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="K158" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="L158" s="9"/>
+      <c r="M158" s="9">
+        <v>2</v>
+      </c>
+      <c r="N158" s="9"/>
+      <c r="O158" s="9">
+        <v>111</v>
+      </c>
+      <c r="P158" s="9">
+        <v>26</v>
+      </c>
+      <c r="Q158" s="9">
+        <v>71</v>
+      </c>
+      <c r="R158" s="9">
+        <v>74</v>
+      </c>
+      <c r="S158" s="9">
+        <v>22</v>
+      </c>
     </row>
     <row r="159" spans="1:19">
       <c r="B159" s="4" t="s">
         <v>219</v>
       </c>
+      <c r="G159" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H159" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="I159" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="J159" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="K159" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="L159" s="12"/>
+      <c r="M159" s="12">
+        <v>0</v>
+      </c>
+      <c r="O159" s="12">
+        <v>143</v>
+      </c>
+      <c r="P159" s="12">
+        <v>25</v>
+      </c>
+      <c r="Q159" s="12">
+        <v>82</v>
+      </c>
+      <c r="R159" s="12">
+        <v>76</v>
+      </c>
+      <c r="S159" s="12">
+        <v>51</v>
+      </c>
     </row>
     <row r="160" spans="1:19">
       <c r="B160" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="161" spans="1:6">
+      <c r="G160" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="H160" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="I160" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="J160" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="K160" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="M160" s="12">
+        <v>1</v>
+      </c>
+      <c r="O160" s="12">
+        <v>136</v>
+      </c>
+      <c r="P160" s="12">
+        <v>35</v>
+      </c>
+      <c r="Q160" s="12">
+        <v>66</v>
+      </c>
+      <c r="R160" s="12">
+        <v>74</v>
+      </c>
+      <c r="S160" s="12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19">
       <c r="B161" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="162" spans="1:6">
+      <c r="G161" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="H161" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="I161" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="J161" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="K161" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="L161" s="12"/>
+      <c r="M161" s="12">
+        <v>0</v>
+      </c>
+      <c r="O161" s="12">
+        <v>185</v>
+      </c>
+      <c r="P161" s="12">
+        <v>31</v>
+      </c>
+      <c r="Q161" s="12">
+        <v>49</v>
+      </c>
+      <c r="R161" s="12">
+        <v>141</v>
+      </c>
+      <c r="S161" s="12">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19">
       <c r="B162" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="163" spans="1:6">
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="9"/>
+      <c r="J162" s="9"/>
+      <c r="K162" s="9"/>
+      <c r="L162" s="9"/>
+      <c r="M162" s="9"/>
+      <c r="N162" s="9"/>
+      <c r="O162" s="9">
+        <f>AVERAGE(O156:O158)</f>
+        <v>90</v>
+      </c>
+      <c r="P162" s="9">
+        <f>AVERAGE(P156:P158)</f>
+        <v>22</v>
+      </c>
+      <c r="Q162" s="9">
+        <v>54</v>
+      </c>
+      <c r="R162" s="9">
+        <v>53</v>
+      </c>
+      <c r="S162" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19">
       <c r="B163" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="165" spans="1:6">
+      <c r="O163">
+        <v>155</v>
+      </c>
+      <c r="P163">
+        <v>30</v>
+      </c>
+      <c r="Q163">
+        <v>66</v>
+      </c>
+      <c r="R163">
+        <f>AVERAGE(R159:R161)</f>
+        <v>97</v>
+      </c>
+      <c r="S163">
+        <f>AVERAGE(S159:S161)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19">
       <c r="A165">
         <v>17</v>
       </c>
@@ -7011,43 +7966,294 @@
       <c r="F165">
         <v>144</v>
       </c>
-    </row>
-    <row r="166" spans="1:6">
+      <c r="G165" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="H165" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I165" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="J165" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="K165" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="L165" s="9"/>
+      <c r="M165" s="9">
+        <v>1</v>
+      </c>
+      <c r="N165" s="9"/>
+      <c r="O165" s="9">
+        <v>125</v>
+      </c>
+      <c r="P165" s="9">
+        <v>41</v>
+      </c>
+      <c r="Q165" s="9">
+        <v>78</v>
+      </c>
+      <c r="R165" s="9">
+        <v>56</v>
+      </c>
+      <c r="S165" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19">
+      <c r="A166" t="s">
+        <v>203</v>
+      </c>
       <c r="B166" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="167" spans="1:6">
+      <c r="G166" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="H166" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="I166" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="J166" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="K166" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="L166" s="9"/>
+      <c r="M166" s="9">
+        <v>0</v>
+      </c>
+      <c r="N166" s="9"/>
+      <c r="O166" s="9">
+        <v>122</v>
+      </c>
+      <c r="P166" s="9">
+        <v>29</v>
+      </c>
+      <c r="Q166" s="9">
+        <v>50</v>
+      </c>
+      <c r="R166" s="9">
+        <v>78</v>
+      </c>
+      <c r="S166" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19">
       <c r="B167" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="168" spans="1:6">
+      <c r="G167" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="H167" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="I167" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J167" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="K167" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="L167" s="9"/>
+      <c r="M167" s="9">
+        <v>0</v>
+      </c>
+      <c r="N167" s="9"/>
+      <c r="O167" s="9">
+        <v>87</v>
+      </c>
+      <c r="P167" s="9">
+        <v>29</v>
+      </c>
+      <c r="Q167" s="9">
+        <v>47</v>
+      </c>
+      <c r="R167" s="9">
+        <v>46</v>
+      </c>
+      <c r="S167" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19">
       <c r="B168" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="169" spans="1:6">
+      <c r="G168" t="s">
+        <v>467</v>
+      </c>
+      <c r="H168" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="I168" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J168" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="K168" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="L168" s="12"/>
+      <c r="M168" s="12">
+        <v>0</v>
+      </c>
+      <c r="O168" s="12">
+        <v>133</v>
+      </c>
+      <c r="P168" s="12">
+        <v>40</v>
+      </c>
+      <c r="Q168" s="12">
+        <v>98</v>
+      </c>
+      <c r="R168" s="12">
+        <v>39</v>
+      </c>
+      <c r="S168" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19">
       <c r="B169" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="170" spans="1:6">
+      <c r="G169" t="s">
+        <v>439</v>
+      </c>
+      <c r="H169" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="I169" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="J169" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="K169" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="L169" s="12"/>
+      <c r="M169" s="12">
+        <v>0</v>
+      </c>
+      <c r="O169" s="12">
+        <v>135</v>
+      </c>
+      <c r="P169" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q169" s="12">
+        <v>51</v>
+      </c>
+      <c r="R169" s="12">
+        <v>93</v>
+      </c>
+      <c r="S169" s="12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19">
       <c r="B170" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="171" spans="1:6">
+      <c r="G170" t="s">
+        <v>32</v>
+      </c>
+      <c r="H170" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="I170" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="J170" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K170" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="L170" s="12"/>
+      <c r="M170" s="12">
+        <v>0</v>
+      </c>
+      <c r="O170" s="12">
+        <v>115</v>
+      </c>
+      <c r="P170" s="12">
+        <v>29</v>
+      </c>
+      <c r="Q170" s="12">
+        <v>44</v>
+      </c>
+      <c r="R170" s="12">
+        <v>71</v>
+      </c>
+      <c r="S170" s="12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19">
       <c r="B171" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="172" spans="1:6">
+      <c r="G171" s="9"/>
+      <c r="H171" s="9"/>
+      <c r="I171" s="9"/>
+      <c r="J171" s="9"/>
+      <c r="K171" s="9"/>
+      <c r="L171" s="9"/>
+      <c r="M171" s="9"/>
+      <c r="N171" s="9"/>
+      <c r="O171" s="9">
+        <v>111</v>
+      </c>
+      <c r="P171" s="9">
+        <f>AVERAGE(P165:P167)</f>
+        <v>33</v>
+      </c>
+      <c r="Q171" s="9">
+        <v>58</v>
+      </c>
+      <c r="R171" s="9">
+        <f>AVERAGE(R165:R167)</f>
+        <v>60</v>
+      </c>
+      <c r="S171" s="9">
+        <f>AVERAGE(S165:S167)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19">
       <c r="B172" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="174" spans="1:6">
+      <c r="O172">
+        <v>173</v>
+      </c>
+      <c r="P172">
+        <v>32</v>
+      </c>
+      <c r="Q172">
+        <v>64</v>
+      </c>
+      <c r="R172">
+        <v>68</v>
+      </c>
+      <c r="S172">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19">
       <c r="A174">
         <v>18</v>
       </c>
@@ -7066,45 +8272,298 @@
       <c r="F174">
         <v>144</v>
       </c>
-    </row>
-    <row r="175" spans="1:6">
+      <c r="G174" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="H174" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="I174" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="J174" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="K174" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="L174" s="9"/>
+      <c r="M174" s="9">
+        <v>1</v>
+      </c>
+      <c r="N174" s="9"/>
+      <c r="O174" s="9">
+        <v>138</v>
+      </c>
+      <c r="P174" s="9">
+        <v>30</v>
+      </c>
+      <c r="Q174" s="9">
+        <v>50</v>
+      </c>
+      <c r="R174" s="9">
+        <v>93</v>
+      </c>
+      <c r="S174" s="9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="175" spans="1:19">
+      <c r="A175" t="s">
+        <v>203</v>
+      </c>
       <c r="B175" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="176" spans="1:6">
+      <c r="G175" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="H175" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="I175" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="J175" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="K175" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="L175" s="9"/>
+      <c r="M175" s="9">
+        <v>0</v>
+      </c>
+      <c r="N175" s="9"/>
+      <c r="O175" s="9">
+        <v>210</v>
+      </c>
+      <c r="P175" s="9">
+        <v>41</v>
+      </c>
+      <c r="Q175" s="9">
+        <v>135</v>
+      </c>
+      <c r="R175" s="9">
+        <v>164</v>
+      </c>
+      <c r="S175" s="9">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19">
       <c r="B176" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="177" spans="1:6">
+      <c r="G176" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="H176" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="I176" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="J176" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="K176" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="L176" s="9"/>
+      <c r="M176" s="9">
+        <v>0</v>
+      </c>
+      <c r="N176" s="9"/>
+      <c r="O176" s="9">
+        <v>195</v>
+      </c>
+      <c r="P176" s="9">
+        <v>32</v>
+      </c>
+      <c r="Q176" s="9">
+        <v>90</v>
+      </c>
+      <c r="R176" s="9">
+        <v>152</v>
+      </c>
+      <c r="S176" s="9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19">
       <c r="B177" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="178" spans="1:6">
+      <c r="G177" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="H177" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="I177" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="J177" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="K177" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="M177" s="12">
+        <v>1</v>
+      </c>
+      <c r="O177" s="12">
+        <v>241</v>
+      </c>
+      <c r="P177" s="12">
+        <v>49</v>
+      </c>
+      <c r="Q177" s="12">
+        <v>128</v>
+      </c>
+      <c r="R177" s="12">
+        <v>140</v>
+      </c>
+      <c r="S177" s="12">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="178" spans="1:19">
       <c r="B178" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="179" spans="1:6">
+      <c r="G178" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="H178" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="I178" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="J178" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="K178" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="L178" s="12"/>
+      <c r="M178" s="12">
+        <v>0</v>
+      </c>
+      <c r="O178" s="12">
+        <v>194</v>
+      </c>
+      <c r="P178" s="12">
+        <v>35</v>
+      </c>
+      <c r="Q178" s="12">
+        <v>122</v>
+      </c>
+      <c r="R178" s="12">
+        <v>137</v>
+      </c>
+      <c r="S178" s="12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19">
       <c r="B179" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="180" spans="1:6">
+      <c r="G179" t="s">
+        <v>465</v>
+      </c>
+      <c r="H179" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="I179" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="J179" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K179" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="M179" s="12">
+        <v>2</v>
+      </c>
+      <c r="O179" s="12">
+        <v>216</v>
+      </c>
+      <c r="P179" s="12">
+        <v>36</v>
+      </c>
+      <c r="Q179" s="12">
+        <v>64</v>
+      </c>
+      <c r="R179" s="12">
+        <v>110</v>
+      </c>
+      <c r="S179" s="12">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19">
       <c r="B180" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="181" spans="1:6">
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+      <c r="I180" s="9"/>
+      <c r="J180" s="9"/>
+      <c r="K180" s="9"/>
+      <c r="L180" s="9"/>
+      <c r="M180" s="9"/>
+      <c r="N180" s="9"/>
+      <c r="O180" s="9">
+        <f>AVERAGE(O174:O176)</f>
+        <v>181</v>
+      </c>
+      <c r="P180" s="9">
+        <v>34</v>
+      </c>
+      <c r="Q180" s="9">
+        <v>92</v>
+      </c>
+      <c r="R180" s="9">
+        <v>136</v>
+      </c>
+      <c r="S180" s="9">
+        <f>AVERAGE(S174:S176)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19">
       <c r="B181" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="183" spans="1:6">
+      <c r="O181">
+        <f>AVERAGE(O177:O179)</f>
+        <v>217</v>
+      </c>
+      <c r="P181">
+        <f>AVERAGE(P177:P179)</f>
+        <v>40</v>
+      </c>
+      <c r="Q181">
+        <f>AVERAGE(Q178+Q177+Q179)</f>
+        <v>314</v>
+      </c>
+      <c r="R181">
+        <f>AVERAGE(R177:R179)</f>
+        <v>129</v>
+      </c>
+      <c r="S181">
+        <f>AVERAGE(S177:S179)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19">
       <c r="A183" s="4">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B183" s="4" t="s">
         <v>12</v>
@@ -7121,9 +8580,46 @@
       <c r="F183" s="4">
         <v>144</v>
       </c>
-    </row>
-    <row r="184" spans="1:6">
-      <c r="A184" s="4"/>
+      <c r="G183" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="H183" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="I183" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="J183" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="K183" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="L183" s="9"/>
+      <c r="M183" s="9">
+        <v>1</v>
+      </c>
+      <c r="N183" s="9"/>
+      <c r="O183" s="9">
+        <v>459</v>
+      </c>
+      <c r="P183" s="9">
+        <v>43</v>
+      </c>
+      <c r="Q183" s="9">
+        <v>254</v>
+      </c>
+      <c r="R183" s="9">
+        <v>409</v>
+      </c>
+      <c r="S183" s="9">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19">
+      <c r="A184" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="B184" s="4" t="s">
         <v>13</v>
       </c>
@@ -7131,8 +8627,43 @@
       <c r="D184" s="4"/>
       <c r="E184" s="4"/>
       <c r="F184" s="4"/>
-    </row>
-    <row r="185" spans="1:6">
+      <c r="G184" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="H184" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="I184" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="J184" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="K184" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="L184" s="9"/>
+      <c r="M184" s="9">
+        <v>0</v>
+      </c>
+      <c r="N184" s="9"/>
+      <c r="O184" s="9">
+        <v>424</v>
+      </c>
+      <c r="P184" s="9">
+        <v>42</v>
+      </c>
+      <c r="Q184" s="9">
+        <v>253</v>
+      </c>
+      <c r="R184" s="9">
+        <v>379</v>
+      </c>
+      <c r="S184" s="9">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19">
       <c r="A185" s="4"/>
       <c r="B185" s="4" t="s">
         <v>14</v>
@@ -7141,8 +8672,43 @@
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
       <c r="F185" s="4"/>
-    </row>
-    <row r="186" spans="1:6">
+      <c r="G185" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="H185" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="I185" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="J185" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="K185" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="L185" s="9"/>
+      <c r="M185" s="9">
+        <v>0</v>
+      </c>
+      <c r="N185" s="9"/>
+      <c r="O185" s="9">
+        <v>518</v>
+      </c>
+      <c r="P185" s="9">
+        <v>59</v>
+      </c>
+      <c r="Q185" s="9">
+        <v>344</v>
+      </c>
+      <c r="R185" s="9">
+        <v>446</v>
+      </c>
+      <c r="S185" s="9">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19">
       <c r="A186" s="4"/>
       <c r="B186" s="4" t="s">
         <v>219</v>
@@ -7151,8 +8717,41 @@
       <c r="D186" s="4"/>
       <c r="E186" s="4"/>
       <c r="F186" s="4"/>
-    </row>
-    <row r="187" spans="1:6">
+      <c r="G186" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="H186" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="I186" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="J186" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="K186" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="M186">
+        <v>2</v>
+      </c>
+      <c r="O186" s="12">
+        <v>400</v>
+      </c>
+      <c r="P186" s="12">
+        <v>46</v>
+      </c>
+      <c r="Q186" s="12">
+        <v>86</v>
+      </c>
+      <c r="R186" s="12">
+        <v>340</v>
+      </c>
+      <c r="S186" s="12">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19">
       <c r="A187" s="4"/>
       <c r="B187" s="4" t="s">
         <v>123</v>
@@ -7161,8 +8760,42 @@
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
       <c r="F187" s="4"/>
-    </row>
-    <row r="188" spans="1:6">
+      <c r="G187" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="H187" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="I187" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="J187" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="K187" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="L187" s="12"/>
+      <c r="M187" s="12">
+        <v>0</v>
+      </c>
+      <c r="O187" s="12">
+        <v>337</v>
+      </c>
+      <c r="P187" s="12">
+        <v>53</v>
+      </c>
+      <c r="Q187" s="12">
+        <v>136</v>
+      </c>
+      <c r="R187" s="12">
+        <v>234</v>
+      </c>
+      <c r="S187" s="12">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="188" spans="1:19">
       <c r="A188" s="4"/>
       <c r="B188" s="4" t="s">
         <v>124</v>
@@ -7171,8 +8804,42 @@
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
       <c r="F188" s="4"/>
-    </row>
-    <row r="189" spans="1:6">
+      <c r="G188" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="H188" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="I188" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="J188" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="K188" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="L188" s="12"/>
+      <c r="M188" s="12">
+        <v>0</v>
+      </c>
+      <c r="O188" s="12">
+        <v>385</v>
+      </c>
+      <c r="P188" s="12">
+        <v>55</v>
+      </c>
+      <c r="Q188" s="12">
+        <v>178</v>
+      </c>
+      <c r="R188" s="12">
+        <v>308</v>
+      </c>
+      <c r="S188" s="12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="189" spans="1:19">
       <c r="A189" s="4"/>
       <c r="B189" s="4" t="s">
         <v>157</v>
@@ -7181,8 +8848,31 @@
       <c r="D189" s="4"/>
       <c r="E189" s="4"/>
       <c r="F189" s="4"/>
-    </row>
-    <row r="190" spans="1:6">
+      <c r="G189" s="9"/>
+      <c r="H189" s="9"/>
+      <c r="I189" s="9"/>
+      <c r="J189" s="9"/>
+      <c r="K189" s="9"/>
+      <c r="L189" s="9"/>
+      <c r="M189" s="9"/>
+      <c r="N189" s="9"/>
+      <c r="O189" s="9">
+        <v>467</v>
+      </c>
+      <c r="P189" s="9">
+        <v>48</v>
+      </c>
+      <c r="Q189" s="9">
+        <v>284</v>
+      </c>
+      <c r="R189" s="9">
+        <v>411</v>
+      </c>
+      <c r="S189" s="9">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="190" spans="1:19">
       <c r="A190" s="4"/>
       <c r="B190" s="4" t="s">
         <v>158</v>
@@ -7191,6 +8881,23 @@
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
       <c r="F190" s="4"/>
+      <c r="O190">
+        <f>AVERAGE(O186:O188)</f>
+        <v>374</v>
+      </c>
+      <c r="P190">
+        <v>51</v>
+      </c>
+      <c r="Q190">
+        <v>133</v>
+      </c>
+      <c r="R190">
+        <f>AVERAGE(R186:R188)</f>
+        <v>294</v>
+      </c>
+      <c r="S190">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7205,18 +8912,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="8" max="8" width="10.83203125" style="6"/>
+    <col min="9" max="9" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>175</v>
       </c>
@@ -7227,19 +8934,23 @@
         <v>177</v>
       </c>
       <c r="E1" t="s">
+        <v>480</v>
+      </c>
+      <c r="F1" t="s">
         <v>178</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>179</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
+      <c r="A2" s="14"/>
       <c r="B2">
         <v>1</v>
       </c>
@@ -7249,19 +8960,21 @@
       <c r="D2">
         <v>200</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>2.6608796296296297E-2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>2.7175925925925926E-2</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>2.7453703703703702E-2</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>2340</v>
       </c>
-      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -7271,66 +8984,75 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>2.0381944444444446E-2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>1.9664351851851853E-2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>1.9502314814814816E-2</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>1715</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="5">
         <v>1761</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="5">
         <v>1699</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="5">
         <v>1685</v>
       </c>
-      <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>6.2268518518518515E-3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>7.5115740740740742E-3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>7.951388888888888E-3</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="I4" s="6">
+        <v>625</v>
+      </c>
+      <c r="J4" s="5">
+        <v>538</v>
+      </c>
+      <c r="K4" s="5">
+        <v>649</v>
+      </c>
+      <c r="L4" s="5">
+        <v>687</v>
+      </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="I5" s="5"/>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -7340,8 +9062,12 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>481</v>
+      </c>
       <c r="B6">
         <v>2</v>
       </c>
@@ -7351,19 +9077,21 @@
       <c r="D6">
         <v>400</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
         <v>5.5370370370370368E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>5.6041666666666663E-2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>5.4050925925925926E-2</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>4755</v>
       </c>
-      <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -7373,72 +9101,75 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>1.9803240740740739E-2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>2.0208333333333335E-2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>1.9710648148148147E-2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>1720</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7" s="5">
         <v>1711</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="5">
         <v>1746</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="5">
         <v>1703</v>
       </c>
-      <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>183</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>3.5567129629629629E-2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>3.5833333333333335E-2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>3.4340277777777782E-2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="6">
+        <v>3045</v>
+      </c>
+      <c r="J8" s="5">
         <v>3073</v>
       </c>
-      <c r="J8" s="5">
+      <c r="K8" s="5">
         <v>3096</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <v>2967</v>
       </c>
-      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="I9" s="5"/>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -7448,8 +9179,12 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" t="s">
+        <v>481</v>
+      </c>
       <c r="B10">
         <v>3</v>
       </c>
@@ -7459,19 +9194,21 @@
       <c r="D10">
         <v>50</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
         <v>2.3750000000000004E-2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>2.0601851851851854E-2</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>2.0405092592592593E-2</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <v>1865</v>
       </c>
-      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -7481,72 +9218,72 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>2.3182870370370371E-2</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>2.0092592592592592E-2</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>1.9907407407407408E-2</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>1814</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="5">
         <v>2003</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="5">
         <v>1736</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="5">
         <v>1720</v>
       </c>
-      <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>183</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>5.6712962962962956E-4</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>5.0925925925925921E-4</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>4.9768518518518521E-4</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>49</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>44</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>43</v>
       </c>
-      <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="I13" s="5"/>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -7556,8 +9293,12 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" t="s">
+        <v>481</v>
+      </c>
       <c r="B14">
         <v>4</v>
       </c>
@@ -7567,19 +9308,21 @@
       <c r="D14">
         <v>100</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
         <v>2.1574074074074075E-2</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>4.0694444444444443E-2</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>2.431712962962963E-2</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>2494</v>
       </c>
-      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -7589,72 +9332,72 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>182</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>1.982638888888889E-2</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>3.8414351851851852E-2</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>2.238425925925926E-2</v>
       </c>
-      <c r="H15" s="6">
+      <c r="I15" s="6">
         <v>2322</v>
       </c>
-      <c r="I15" s="5">
+      <c r="J15" s="5">
         <v>1713</v>
       </c>
-      <c r="J15" s="5">
+      <c r="K15" s="5">
         <v>3319</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="5">
         <v>1934</v>
       </c>
-      <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>183</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>1.7476851851851852E-3</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>2.2800925925925927E-3</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>1.9328703703703704E-3</v>
       </c>
-      <c r="I16" s="5">
+      <c r="J16" s="5">
         <v>151</v>
       </c>
-      <c r="J16" s="5">
+      <c r="K16" s="5">
         <v>197</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>167</v>
       </c>
-      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="I17" s="5"/>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -7664,8 +9407,10 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="14"/>
       <c r="B18">
         <v>5</v>
       </c>
@@ -7675,19 +9420,21 @@
       <c r="D18">
         <v>200</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
         <v>3.425925925925926E-3</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>2.8703703703703708E-3</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>2.8472222222222219E-3</v>
       </c>
-      <c r="H18" s="6">
+      <c r="I18" s="6">
         <v>263</v>
       </c>
-      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -7697,75 +9444,75 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>182</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>2.4537037037037036E-3</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>1.8518518518518517E-3</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>1.8634259259259261E-3</v>
       </c>
-      <c r="H19" s="6">
+      <c r="I19" s="6">
         <v>178</v>
       </c>
-      <c r="I19" s="5">
+      <c r="J19" s="5">
         <v>212</v>
       </c>
-      <c r="J19" s="5">
+      <c r="K19" s="5">
         <v>160</v>
       </c>
-      <c r="K19" s="5">
+      <c r="L19" s="5">
         <v>161</v>
       </c>
-      <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>183</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>9.7222222222222209E-4</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>1.0185185185185186E-3</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>9.8379629629629642E-4</v>
       </c>
-      <c r="H20" s="6">
+      <c r="I20" s="6">
         <v>86</v>
       </c>
-      <c r="I20" s="5">
+      <c r="J20" s="5">
         <v>84</v>
       </c>
-      <c r="J20" s="5">
+      <c r="K20" s="5">
         <v>88</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L20" s="5">
         <v>85</v>
       </c>
-      <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="I21" s="5"/>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -7775,8 +9522,10 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="14"/>
       <c r="B22">
         <v>6</v>
       </c>
@@ -7786,19 +9535,21 @@
       <c r="D22">
         <v>200</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
         <v>8.5879629629629622E-3</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>7.1643518518518514E-3</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>7.0949074074074074E-3</v>
       </c>
-      <c r="H22" s="6">
+      <c r="I22" s="6">
         <v>658</v>
       </c>
-      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -7808,75 +9559,75 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>182</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>6.1574074074074074E-3</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>4.6759259259259263E-3</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>4.6527777777777774E-3</v>
       </c>
-      <c r="H23" s="6">
+      <c r="I23" s="6">
         <v>446</v>
       </c>
-      <c r="I23" s="5">
+      <c r="J23" s="5">
         <v>532</v>
       </c>
-      <c r="J23" s="5">
+      <c r="K23" s="5">
         <v>404</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="5">
         <v>402</v>
       </c>
-      <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="S23" s="5"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>183</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>2.4305555555555556E-3</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>2.488425925925926E-3</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>2.4421296296296296E-3</v>
       </c>
-      <c r="H24" s="6">
+      <c r="I24" s="6">
         <v>212</v>
       </c>
-      <c r="I24" s="5">
+      <c r="J24" s="5">
         <v>210</v>
       </c>
-      <c r="J24" s="5">
+      <c r="K24" s="5">
         <v>215</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="5">
         <v>211</v>
       </c>
-      <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
-    </row>
-    <row r="25" spans="1:18">
-      <c r="I25" s="5"/>
+      <c r="S24" s="5"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -7886,8 +9637,10 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="S25" s="5"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="14"/>
       <c r="B26">
         <v>7</v>
       </c>
@@ -7897,103 +9650,105 @@
       <c r="D26">
         <v>200</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
         <v>1.6284722222222221E-2</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>1.4791666666666668E-2</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>1.5023148148148148E-2</v>
       </c>
-      <c r="H26" s="6">
+      <c r="I26" s="6">
         <v>1328</v>
       </c>
-      <c r="I26" s="5">
+      <c r="J26" s="5">
         <v>1407</v>
       </c>
-      <c r="J26" s="5">
+      <c r="K26" s="5">
         <v>1278</v>
       </c>
-      <c r="K26" s="5">
+      <c r="L26" s="5">
         <v>1298</v>
       </c>
-      <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>182</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <v>1.091435185185185E-2</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>9.6874999999999999E-3</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>9.6643518518518511E-3</v>
       </c>
-      <c r="H27" s="6">
+      <c r="I27" s="6">
         <v>872</v>
       </c>
-      <c r="I27" s="5">
+      <c r="J27" s="5">
         <v>943</v>
       </c>
-      <c r="J27" s="5">
+      <c r="K27" s="5">
         <v>837</v>
       </c>
-      <c r="K27" s="5">
+      <c r="L27" s="5">
         <v>835</v>
       </c>
-      <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="S27" s="5"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>183</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>5.37037037037037E-3</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>5.1041666666666666E-3</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>5.3587962962962964E-3</v>
       </c>
-      <c r="H28" s="6">
+      <c r="I28" s="6">
         <v>456</v>
       </c>
-      <c r="I28" s="5">
+      <c r="J28" s="5">
         <v>464</v>
       </c>
-      <c r="J28" s="5">
+      <c r="K28" s="5">
         <v>441</v>
       </c>
-      <c r="K28" s="5">
+      <c r="L28" s="5">
         <v>463</v>
       </c>
-      <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="I29" s="5"/>
+      <c r="S28" s="5"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -8003,78 +9758,202 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="S29" s="5"/>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="14"/>
       <c r="B30">
         <v>8</v>
       </c>
       <c r="C30">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="D30">
         <v>200</v>
       </c>
-      <c r="E30" t="s">
-        <v>181</v>
-      </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
+      <c r="E30">
+        <v>200</v>
+      </c>
+      <c r="F30" s="2">
+        <v>3.0474537037037036E-2</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2.9571759259259259E-2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>2.7615740740740743E-2</v>
+      </c>
+      <c r="I30" s="6">
+        <v>2525</v>
+      </c>
+      <c r="J30" s="5">
+        <v>2633</v>
+      </c>
+      <c r="K30" s="5">
+        <v>2555</v>
+      </c>
+      <c r="L30" s="5">
+        <v>2386</v>
+      </c>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="S30" s="5"/>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>182</v>
       </c>
-      <c r="E31" t="s">
-        <v>181</v>
-      </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="F31" s="2">
+        <v>2.2569444444444444E-2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2.164351851851852E-2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1.9861111111111111E-2</v>
+      </c>
+      <c r="I31" s="6">
+        <v>1845</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1950</v>
+      </c>
+      <c r="K31" s="5">
+        <v>1870</v>
+      </c>
+      <c r="L31" s="5">
+        <v>1716</v>
+      </c>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>183</v>
       </c>
-      <c r="E32" t="s">
-        <v>181</v>
-      </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-    </row>
-    <row r="33" spans="9:12">
-      <c r="I33" s="5"/>
+      <c r="F32" s="2">
+        <v>7.905092592592592E-3</v>
+      </c>
+      <c r="G32" s="2">
+        <v>7.9282407407407409E-3</v>
+      </c>
+      <c r="H32" s="2">
+        <v>7.7546296296296287E-3</v>
+      </c>
+      <c r="I32" s="6">
+        <v>679</v>
+      </c>
+      <c r="J32" s="5">
+        <v>683</v>
+      </c>
+      <c r="K32" s="5">
+        <v>685</v>
+      </c>
+      <c r="L32" s="5">
+        <v>670</v>
+      </c>
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-    </row>
-    <row r="34" spans="9:12">
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-    </row>
-    <row r="35" spans="9:12">
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-    </row>
-    <row r="36" spans="9:12">
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="14"/>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>150</v>
+      </c>
+      <c r="D34">
+        <v>100</v>
+      </c>
+      <c r="E34">
+        <v>200</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2.2870370370370371E-2</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2.2962962962962966E-2</v>
+      </c>
+      <c r="I34" s="6">
+        <f>AVERAGE(J34:L34)</f>
+        <v>2000</v>
+      </c>
+      <c r="J34" s="5">
+        <v>1976</v>
+      </c>
+      <c r="K34" s="5">
+        <v>2040</v>
+      </c>
+      <c r="L34" s="5">
+        <v>1984</v>
+      </c>
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+      <c r="F35" s="2">
+        <v>2.0983796296296296E-2</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2.179398148148148E-2</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2.1134259259259259E-2</v>
+      </c>
+      <c r="I35" s="6">
+        <v>1841</v>
+      </c>
+      <c r="J35" s="5">
+        <v>1813</v>
+      </c>
+      <c r="K35" s="5">
+        <v>1883</v>
+      </c>
+      <c r="L35" s="5">
+        <v>1826</v>
+      </c>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" t="s">
+        <v>183</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1.8865740740740742E-3</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1.8171296296296297E-3</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1.8287037037037037E-3</v>
+      </c>
+      <c r="I36" s="6">
+        <v>159</v>
+      </c>
+      <c r="J36" s="5">
+        <v>163</v>
+      </c>
+      <c r="K36" s="5">
+        <v>157</v>
+      </c>
+      <c r="L36" s="5">
+        <v>158</v>
+      </c>
+      <c r="M36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>